<commit_message>
Worked on lots of data analysis and simulations
</commit_message>
<xml_diff>
--- a/Other files/Pacientes_sinais2e10.xlsx
+++ b/Other files/Pacientes_sinais2e10.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="28755" windowHeight="12600" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="28755" windowHeight="12600" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,11 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$A$25:$B$26</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="104">
   <si>
     <t>Código</t>
   </si>
@@ -294,13 +293,56 @@
   <si>
     <t>10 - Gord B - S/tan</t>
   </si>
+  <si>
+    <t>A=</t>
+  </si>
+  <si>
+    <t>B=</t>
+  </si>
+  <si>
+    <t>2 norm</t>
+  </si>
+  <si>
+    <t>10 norm</t>
+  </si>
+  <si>
+    <t>Angle</t>
+  </si>
+  <si>
+    <t>sin</t>
+  </si>
+  <si>
+    <t>cos</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>gamma</t>
+  </si>
+  <si>
+    <t>T1 norm</t>
+  </si>
+  <si>
+    <t>gamma norm</t>
+  </si>
+  <si>
+    <t>STDEV</t>
+  </si>
+  <si>
+    <t>AVG</t>
+  </si>
+  <si>
+    <t>SNR</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="170" formatCode="0.00000"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -391,7 +433,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -430,6 +472,15 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -437,40 +488,30 @@
     <cellStyle name="Input" xfId="3" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="141">
+  <dxfs count="143">
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -957,6 +998,40 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -1712,49 +1787,1567 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pt-BR"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Original!$F$2:$F$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>48.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>103.07</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>98.83</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>105.24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>81.55</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>147.11000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100.67</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>105.4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>129.22</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>114.62</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>137.38999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>106.07</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>114.83</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>121.84</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>84.77</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>82.56</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>73.17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>147.34</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>128.65</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>77.239999999999995</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>118.07</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>82.52</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Original!$G$2:$G$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="23"/>
+                <c:pt idx="0">
+                  <c:v>192.36</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>263.39999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>207.39</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>253.36</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>168.21</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>293.20999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>200.36</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>233.16</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>297.52999999999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>251.15</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>275.77999999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>212.25</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>252.66</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>283.60000000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>185.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>189.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>155.74</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>504.11</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>247.62</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>175.29</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>252.44</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>177.48</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>1x</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Original!$T$2:$T$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>160</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Original!$T$2:$T$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>160</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>A*x</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Original!$T$2:$T$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>160</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Original!$U$2:$U$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>320</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>B*x</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Original!$T$2:$T$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>160</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Original!$V$2:$V$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>480</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="77041024"/>
+        <c:axId val="77039488"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="77041024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="77039488"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="77039488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="77041024"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pt-BR"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Rescaled!$B$2:$B$23</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>3.275167785234899</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.490523968784837</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.8557347670250888</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.6373626373626369</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.3270440251572317</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20.40360610263523</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.710858585858587</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10.810256410256411</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>17.67715458276334</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>12.864197530864198</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14.998908296943229</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10.258220502901354</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.138443935926773</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12.319514661274013</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7.9821092278719403</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.6000000000000014</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.0271828665568368</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>21.2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>16.101376720901126</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.7399650959860375</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>14.703611457036114</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>7.996124031007751</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Rescaled!$C$2:$C$23</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>37.717647058823538</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>49.698113207547166</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41.8125</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42.510067114093964</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>35.338235294117652</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>67.559907834101381</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>34.845217391304352</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>46.91348088531187</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>79.766756032171571</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45.998168498168496</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>105.25954198473281</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>43.316326530612244</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>60.157142857142851</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>55.175097276264601</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>31.387478849407781</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>32.173174872665534</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>21.189115646258507</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>254.6010101010101</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>51.16115702479339</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>27.604724409448821</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>73.597667638483955</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>30.030456852791875</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>1x</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Rescaled!$P$2:$P$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Rescaled!$P$2:$P$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>A*x</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Rescaled!$P$2:$P$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Rescaled!$Q$2:$Q$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>4.74</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.48</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18.96</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>23.700000000000003</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>28.44</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33.18</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>37.92</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42.660000000000004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>47.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>52.14</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>56.88</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>66.36</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>71.100000000000009</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>75.84</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>80.58</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>85.320000000000007</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>90.06</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>94.800000000000011</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="101579008"/>
+        <c:axId val="81543168"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="101579008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="81543168"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="81543168"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="101579008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pt-BR"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Rescaled!$M$27:$M$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Rescaled!$N$27:$N$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="1">
+                  <c:v>4.3251389877917736</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.7215167459273504</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.4109647746665344</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.8229866195405213</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.311174872434715</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.7413740115141598</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.3397195316109176</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.5124205741771721</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.5756733669401615</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.2225965525269222</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.5787113870193199</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.4786745901367118</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.9322286820893075</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.7410668456587826</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.5155919631758685</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.1774399116059011</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.0956776505992174</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.7556266931751354</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>T1</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Rescaled!$W$27:$W$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="1">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Rescaled!$S$28:$S$47</c:f>
+              <c:numCache>
+                <c:formatCode>0.00000</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1.7611436189939353</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.67707794546015254</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5093617935882735</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4280301934750958</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.7846483968471025</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.4538129635987005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.7176378536963226</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.2245488615868034</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.5022730604685011</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.0759804104281954</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0454877302132917</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.3177997023817716</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.0610911009201853</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.7976968502088377</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.7756156281657471</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.519728458894841</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.488538187070489</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.7388090681306001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="82361344"/>
+        <c:axId val="82372096"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="82361344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="82372096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="82372096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="82361344"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>304799</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>47624</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q23" totalsRowShown="0" headerRowDxfId="140" dataDxfId="139">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q23" totalsRowShown="0" headerRowDxfId="142" dataDxfId="141">
   <tableColumns count="17">
-    <tableColumn id="2" name="Código" dataDxfId="138"/>
-    <tableColumn id="16" name="Rescale A_2" dataDxfId="137"/>
-    <tableColumn id="17" name="Rescale B_2" dataDxfId="136"/>
-    <tableColumn id="18" name="Rescale A_10" dataDxfId="135"/>
-    <tableColumn id="19" name="Rescale B_10" dataDxfId="134"/>
-    <tableColumn id="1" name="2 - Fígado A" dataDxfId="133"/>
-    <tableColumn id="3" name="10 - Fígado A" dataDxfId="132"/>
-    <tableColumn id="4" name="2 - Fígado B" dataDxfId="131"/>
-    <tableColumn id="5" name="10 - Fígado B" dataDxfId="130"/>
-    <tableColumn id="6" name="2 - Fígado C" dataDxfId="129"/>
-    <tableColumn id="7" name="10 - Fígado C" dataDxfId="128"/>
-    <tableColumn id="8" name="2 - Rim " dataDxfId="127"/>
-    <tableColumn id="9" name="10 - Rim" dataDxfId="126"/>
-    <tableColumn id="10" name="2 - Gordura A" dataDxfId="125"/>
-    <tableColumn id="11" name="10 - Gordura A" dataDxfId="124"/>
-    <tableColumn id="12" name="2 - Gordura B" dataDxfId="123"/>
-    <tableColumn id="13" name="10 - Gordura B" dataDxfId="122"/>
+    <tableColumn id="2" name="Código" dataDxfId="140"/>
+    <tableColumn id="16" name="Rescale A_2" dataDxfId="139"/>
+    <tableColumn id="17" name="Rescale B_2" dataDxfId="138"/>
+    <tableColumn id="18" name="Rescale A_10" dataDxfId="137"/>
+    <tableColumn id="19" name="Rescale B_10" dataDxfId="136"/>
+    <tableColumn id="1" name="2 - Fígado A" dataDxfId="135"/>
+    <tableColumn id="3" name="10 - Fígado A" dataDxfId="134"/>
+    <tableColumn id="4" name="2 - Fígado B" dataDxfId="133"/>
+    <tableColumn id="5" name="10 - Fígado B" dataDxfId="132"/>
+    <tableColumn id="6" name="2 - Fígado C" dataDxfId="131"/>
+    <tableColumn id="7" name="10 - Fígado C" dataDxfId="130"/>
+    <tableColumn id="8" name="2 - Rim " dataDxfId="129"/>
+    <tableColumn id="9" name="10 - Rim" dataDxfId="128"/>
+    <tableColumn id="10" name="2 - Gordura A" dataDxfId="127"/>
+    <tableColumn id="11" name="10 - Gordura A" dataDxfId="126"/>
+    <tableColumn id="12" name="2 - Gordura B" dataDxfId="125"/>
+    <tableColumn id="13" name="10 - Gordura B" dataDxfId="124"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table511" displayName="Table511" ref="K2:Q20" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table511" displayName="Table511" ref="K2:Q20" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="K2:Q20"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Paciente" dataDxfId="15"/>
-    <tableColumn id="2" name="Fígado A" dataDxfId="14"/>
-    <tableColumn id="3" name="Fígado B" dataDxfId="13"/>
-    <tableColumn id="4" name="Fígado C" dataDxfId="12"/>
-    <tableColumn id="5" name="Rim" dataDxfId="11"/>
-    <tableColumn id="6" name="Gordura A" dataDxfId="10"/>
-    <tableColumn id="7" name="Gordura B" dataDxfId="9"/>
+    <tableColumn id="1" name="Paciente" dataDxfId="8"/>
+    <tableColumn id="2" name="Fígado A" dataDxfId="7"/>
+    <tableColumn id="3" name="Fígado B" dataDxfId="6"/>
+    <tableColumn id="4" name="Fígado C" dataDxfId="5"/>
+    <tableColumn id="5" name="Rim" dataDxfId="4"/>
+    <tableColumn id="6" name="Gordura A" dataDxfId="3"/>
+    <tableColumn id="7" name="Gordura B" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:M23" totalsRowShown="0" headerRowDxfId="121" dataDxfId="120">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:M23" totalsRowShown="0" headerRowDxfId="123" dataDxfId="122">
   <autoFilter ref="A1:M23">
     <filterColumn colId="1"/>
     <filterColumn colId="2"/>
@@ -1770,41 +3363,41 @@
     <filterColumn colId="12"/>
   </autoFilter>
   <tableColumns count="13">
-    <tableColumn id="1" name="Código" dataDxfId="119"/>
-    <tableColumn id="2" name="2 - Fígado A" dataDxfId="118">
+    <tableColumn id="1" name="Código" dataDxfId="121"/>
+    <tableColumn id="2" name="2 - Fígado A" dataDxfId="120">
       <calculatedColumnFormula>Table1[[#This Row],[2 - Fígado A]]/Table1[[#This Row],[Rescale A_2]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="10 - Fígado A" dataDxfId="117">
+    <tableColumn id="3" name="10 - Fígado A" dataDxfId="119">
       <calculatedColumnFormula>Table1[[#This Row],[10 - Fígado A]]/Table1[[#This Row],[Rescale A_10]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="2 - Fígado B" dataDxfId="116">
+    <tableColumn id="7" name="2 - Fígado B" dataDxfId="118">
       <calculatedColumnFormula>Table1[[#This Row],[2 - Fígado B]]/Table1[[#This Row],[Rescale A_2]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="10 - Fígado B" dataDxfId="115">
+    <tableColumn id="8" name="10 - Fígado B" dataDxfId="117">
       <calculatedColumnFormula>Table1[[#This Row],[10 - Fígado B]]/Table1[[#This Row],[Rescale A_10]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="2 - Fígado C" dataDxfId="114">
+    <tableColumn id="9" name="2 - Fígado C" dataDxfId="116">
       <calculatedColumnFormula>Table1[[#This Row],[2 - Fígado C]]/Table1[[#This Row],[Rescale A_2]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="10 - Fígado C" dataDxfId="113">
+    <tableColumn id="10" name="10 - Fígado C" dataDxfId="115">
       <calculatedColumnFormula>Table1[[#This Row],[10 - Fígado C]]/Table1[[#This Row],[Rescale A_10]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="2 - Rim " dataDxfId="112">
+    <tableColumn id="11" name="2 - Rim " dataDxfId="114">
       <calculatedColumnFormula>Table1[[#This Row],[2 - Rim ]]/Table1[[#This Row],[Rescale A_2]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="10 - Rim" dataDxfId="111">
+    <tableColumn id="12" name="10 - Rim" dataDxfId="113">
       <calculatedColumnFormula>Table1[[#This Row],[10 - Rim]]/Table1[[#This Row],[Rescale A_10]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="2 - Gordura A" dataDxfId="110">
+    <tableColumn id="13" name="2 - Gordura A" dataDxfId="112">
       <calculatedColumnFormula>Table1[[#This Row],[2 - Gordura A]]/Table1[[#This Row],[Rescale A_2]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="10 - Gordura A" dataDxfId="109">
+    <tableColumn id="14" name="10 - Gordura A" dataDxfId="111">
       <calculatedColumnFormula>Table1[[#This Row],[10 - Gordura A]]/Table1[[#This Row],[Rescale A_10]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="2 - Gordura B" dataDxfId="108">
+    <tableColumn id="15" name="2 - Gordura B" dataDxfId="110">
       <calculatedColumnFormula>Table1[[#This Row],[2 - Gordura B]]/Table1[[#This Row],[Rescale A_2]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="10 - Gordura B" dataDxfId="107">
+    <tableColumn id="16" name="10 - Gordura B" dataDxfId="109">
       <calculatedColumnFormula>Table1[[#This Row],[10 - Gordura B]]/Table1[[#This Row],[Rescale A_10]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1813,79 +3406,79 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table11" displayName="Table11" ref="A1:Y23" totalsRowShown="0" headerRowDxfId="93" dataDxfId="92">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table11" displayName="Table11" ref="A1:Y23" totalsRowShown="0" headerRowDxfId="95" dataDxfId="94">
   <tableColumns count="25">
-    <tableColumn id="1" name="Código" dataDxfId="91"/>
-    <tableColumn id="2" name="2 - Fíg A - S/sin" dataDxfId="90">
+    <tableColumn id="1" name="Código" dataDxfId="93"/>
+    <tableColumn id="2" name="2 - Fíg A - S/sin" dataDxfId="92">
       <calculatedColumnFormula>Table4[[#This Row],[2 - Fígado A]]/SIN(Original!$B$25*PI()/180)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="10 - Fíg A - S/sin" dataDxfId="89">
+    <tableColumn id="3" name="10 - Fíg A - S/sin" dataDxfId="91">
       <calculatedColumnFormula>Table4[[#This Row],[10 - Fígado A]]/SIN(Original!$B$26*PI()/180)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="2 - Fíg A - S/tan" dataDxfId="88">
+    <tableColumn id="14" name="2 - Fíg A - S/tan" dataDxfId="90">
       <calculatedColumnFormula>Table4[[#This Row],[2 - Fígado A]]/TAN(Original!$B$25*PI()/180)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="10 - Fíg A - S/tan" dataDxfId="87">
+    <tableColumn id="15" name="10 - Fíg A - S/tan" dataDxfId="89">
       <calculatedColumnFormula>Table4[[#This Row],[10 - Fígado A]]/TAN(Original!$B$26*PI()/180)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="2 - Fíg B - S/sin" dataDxfId="86">
+    <tableColumn id="4" name="2 - Fíg B - S/sin" dataDxfId="88">
       <calculatedColumnFormula>Table4[[#This Row],[2 - Fígado B]]/SIN(Original!$B$25*PI()/180)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="10 - Fíg B - S/sin" dataDxfId="85">
+    <tableColumn id="5" name="10 - Fíg B - S/sin" dataDxfId="87">
       <calculatedColumnFormula>Table4[[#This Row],[10 - Fígado B]]/SIN(Original!$B$26*PI()/180)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="2 - Fíg B - S/tan" dataDxfId="84">
+    <tableColumn id="6" name="2 - Fíg B - S/tan" dataDxfId="86">
       <calculatedColumnFormula>Table4[[#This Row],[2 - Fígado B]]/TAN(Original!$B$25*PI()/180)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="10 - Fíg B - S/tan" dataDxfId="83">
+    <tableColumn id="7" name="10 - Fíg B - S/tan" dataDxfId="85">
       <calculatedColumnFormula>Table4[[#This Row],[10 - Fígado B]]/TAN(Original!$B$26*PI()/180)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="2 - Fíg C - S/sin" dataDxfId="82">
+    <tableColumn id="8" name="2 - Fíg C - S/sin" dataDxfId="84">
       <calculatedColumnFormula>Table4[[#This Row],[2 - Fígado C]]/SIN(Original!$B$25*PI()/180)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="10 - Fíg C - S/sin" dataDxfId="81">
+    <tableColumn id="9" name="10 - Fíg C - S/sin" dataDxfId="83">
       <calculatedColumnFormula>Table4[[#This Row],[10 - Fígado C]]/SIN(Original!$B$26*PI()/180)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="2 - Fíg C - S/tan" dataDxfId="80">
+    <tableColumn id="10" name="2 - Fíg C - S/tan" dataDxfId="82">
       <calculatedColumnFormula>Table4[[#This Row],[2 - Fígado C]]/TAN(Original!$B$25*PI()/180)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="10 - Fíg C - S/tan" dataDxfId="79">
+    <tableColumn id="11" name="10 - Fíg C - S/tan" dataDxfId="81">
       <calculatedColumnFormula>Table4[[#This Row],[10 - Fígado C]]/TAN(Original!$B$26*PI()/180)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="2 - Rim - S/sin" dataDxfId="78">
+    <tableColumn id="16" name="2 - Rim - S/sin" dataDxfId="80">
       <calculatedColumnFormula>Table4[[#This Row],[2 - Rim ]]/SIN(Original!$B$25*PI()/180)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="10 - Rim - S/sin" dataDxfId="77">
+    <tableColumn id="17" name="10 - Rim - S/sin" dataDxfId="79">
       <calculatedColumnFormula>Table4[[#This Row],[10 - Rim]]/SIN(Original!$B$26*PI()/180)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="2 - Rim - S/tan" dataDxfId="76">
+    <tableColumn id="18" name="2 - Rim - S/tan" dataDxfId="78">
       <calculatedColumnFormula>Table4[[#This Row],[2 - Rim ]]/TAN(Original!$B$25*PI()/180)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="10 - Rim - S/tan" dataDxfId="75">
+    <tableColumn id="19" name="10 - Rim - S/tan" dataDxfId="77">
       <calculatedColumnFormula>Table4[[#This Row],[10 - Rim]]/TAN(Original!$B$26*PI()/180)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" name="2 - Gord A - S/sin" dataDxfId="74">
+    <tableColumn id="20" name="2 - Gord A - S/sin" dataDxfId="76">
       <calculatedColumnFormula>Table4[[#This Row],[2 - Gordura A]]/SIN(Original!$B$25*PI()/180)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="10 - Gord A - S/sin" dataDxfId="73">
+    <tableColumn id="21" name="10 - Gord A - S/sin" dataDxfId="75">
       <calculatedColumnFormula>Table4[[#This Row],[10 - Gordura A]]/SIN(Original!$B$26*PI()/180)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" name="2 - Gord A - S/tan" dataDxfId="72">
+    <tableColumn id="22" name="2 - Gord A - S/tan" dataDxfId="74">
       <calculatedColumnFormula>Table4[[#This Row],[2 - Gordura A]]/TAN(Original!$B$25*PI()/180)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" name="10 - Gord A - S/tan" dataDxfId="71">
+    <tableColumn id="23" name="10 - Gord A - S/tan" dataDxfId="73">
       <calculatedColumnFormula>Table4[[#This Row],[10 - Gordura A]]/TAN(Original!$B$26*PI()/180)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" name="2 - Gord B - S/sin" dataDxfId="70">
+    <tableColumn id="24" name="2 - Gord B - S/sin" dataDxfId="72">
       <calculatedColumnFormula>Table4[[#This Row],[2 - Gordura B]]/SIN(Original!$B$25*PI()/180)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" name="10 - Gord B - S/sin" dataDxfId="69">
+    <tableColumn id="25" name="10 - Gord B - S/sin" dataDxfId="71">
       <calculatedColumnFormula>Table4[[#This Row],[10 - Gordura B]]/SIN(Original!$B$26*PI()/180)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" name="2 - Gord B - S/tan" dataDxfId="68">
+    <tableColumn id="26" name="2 - Gord B - S/tan" dataDxfId="70">
       <calculatedColumnFormula>Table4[[#This Row],[2 - Gordura B]]/TAN(Original!$B$25*PI()/180)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" name="10 - Gord B - S/tan" dataDxfId="67">
+    <tableColumn id="27" name="10 - Gord B - S/tan" dataDxfId="69">
       <calculatedColumnFormula>Table4[[#This Row],[10 - Gordura B]]/TAN(Original!$B$26*PI()/180)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1894,26 +3487,26 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="AC1:AI23" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="AC1:AI23" totalsRowShown="0" headerRowDxfId="68" dataDxfId="67">
   <autoFilter ref="AC1:AI23"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Código" dataDxfId="8"/>
-    <tableColumn id="2" name="T1 Fig A" dataDxfId="7">
+    <tableColumn id="1" name="Código" dataDxfId="66"/>
+    <tableColumn id="2" name="T1 Fig A" dataDxfId="65">
       <calculatedColumnFormula>-$B$26/LN((Table11[[#This Row],[2 - Fíg A - S/sin]]-Table11[[#This Row],[10 - Fíg A - S/sin]])/(Table11[[#This Row],[2 - Fíg A - S/tan]]-Table11[[#This Row],[10 - Fíg A - S/tan]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="T1 Fig B" dataDxfId="6">
+    <tableColumn id="3" name="T1 Fig B" dataDxfId="64">
       <calculatedColumnFormula>-$B$26/LN((Table11[[#This Row],[2 - Fíg B - S/sin]]-Table11[[#This Row],[10 - Fíg B - S/sin]])/(Table11[[#This Row],[2 - Fíg B - S/tan]]-Table11[[#This Row],[10 - Fíg B - S/tan]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="T1 Fig C" dataDxfId="5">
+    <tableColumn id="4" name="T1 Fig C" dataDxfId="63">
       <calculatedColumnFormula>-$B$26/LN((Table11[[#This Row],[2 - Fíg C - S/sin]]-Table11[[#This Row],[10 - Fíg C - S/sin]])/(Table11[[#This Row],[2 - Fíg C - S/tan]]-Table11[[#This Row],[10 - Fíg C - S/tan]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="T1 Rim" dataDxfId="4">
+    <tableColumn id="5" name="T1 Rim" dataDxfId="62">
       <calculatedColumnFormula>-$B$26/LN((N2-O2)/(P2-Q2))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="T1 Gord. A" dataDxfId="3">
+    <tableColumn id="6" name="T1 Gord. A" dataDxfId="61">
       <calculatedColumnFormula>-$B$26/LN((Table11[[#This Row],[2 - Gord B - S/sin]]-Table11[[#This Row],[10 - Gord B - S/sin]])/(Table11[[#This Row],[2 - Gord B - S/tan]]-Table11[[#This Row],[10 - Gord B - S/tan]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="T1 Gord. B" dataDxfId="2">
+    <tableColumn id="7" name="T1 Gord. B" dataDxfId="60">
       <calculatedColumnFormula>-$B$26/LN((V2-W2)/(X2-Y2))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1922,25 +3515,25 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A2:G24" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A2:G24" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
   <tableColumns count="7">
-    <tableColumn id="1" name="Paciente" dataDxfId="64"/>
-    <tableColumn id="2" name="Fígado A" dataDxfId="63">
+    <tableColumn id="1" name="Paciente" dataDxfId="57"/>
+    <tableColumn id="2" name="Fígado A" dataDxfId="56">
       <calculatedColumnFormula>(Rescaled!C2-Rescaled!B2)/(Original!$B$26-Original!$B$25)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Fígado B" dataDxfId="62">
+    <tableColumn id="3" name="Fígado B" dataDxfId="55">
       <calculatedColumnFormula>(Rescaled!E2-Rescaled!D2)/(Original!$B$26-Original!$B$25)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Fígado C" dataDxfId="61">
+    <tableColumn id="4" name="Fígado C" dataDxfId="54">
       <calculatedColumnFormula>(Rescaled!G2-Rescaled!F2)/(Original!$B$26-Original!$B$25)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Rim" dataDxfId="60">
+    <tableColumn id="5" name="Rim" dataDxfId="53">
       <calculatedColumnFormula>(Rescaled!I2-Rescaled!H2)/(Original!$B$26-Original!$B$25)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Gordura A" dataDxfId="59">
+    <tableColumn id="6" name="Gordura A" dataDxfId="52">
       <calculatedColumnFormula>(Rescaled!K2-Rescaled!J2)/(Original!$B$26-Original!$B$25)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Gordura B" dataDxfId="58">
+    <tableColumn id="7" name="Gordura B" dataDxfId="51">
       <calculatedColumnFormula>(Rescaled!M2-Rescaled!L2)/(Original!$B$26-Original!$B$25)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1949,59 +3542,59 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="K2:Q22" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="K2:Q22" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49">
   <autoFilter ref="K2:Q22"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Paciente" dataDxfId="55"/>
-    <tableColumn id="2" name="Fígado A" dataDxfId="54"/>
-    <tableColumn id="3" name="Fígado B" dataDxfId="53"/>
-    <tableColumn id="4" name="Fígado C" dataDxfId="52"/>
-    <tableColumn id="5" name="Rim" dataDxfId="51"/>
-    <tableColumn id="6" name="Gordura A" dataDxfId="50"/>
-    <tableColumn id="7" name="Gordura B" dataDxfId="49"/>
+    <tableColumn id="1" name="Paciente" dataDxfId="48"/>
+    <tableColumn id="2" name="Fígado A" dataDxfId="47"/>
+    <tableColumn id="3" name="Fígado B" dataDxfId="46"/>
+    <tableColumn id="4" name="Fígado C" dataDxfId="45"/>
+    <tableColumn id="5" name="Rim" dataDxfId="44"/>
+    <tableColumn id="6" name="Gordura A" dataDxfId="43"/>
+    <tableColumn id="7" name="Gordura B" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table43" displayName="Table43" ref="A1:M23" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table43" displayName="Table43" ref="A1:M23" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
   <tableColumns count="13">
-    <tableColumn id="1" name="Código" dataDxfId="46"/>
-    <tableColumn id="2" name="2 - Fígado A" dataDxfId="45">
+    <tableColumn id="1" name="Código" dataDxfId="39"/>
+    <tableColumn id="2" name="2 - Fígado A" dataDxfId="38">
       <calculatedColumnFormula>Table1[[#This Row],[2 - Fígado A]]/Table1[[#This Row],[Rescale A_2]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="10 - Fígado A" dataDxfId="44">
+    <tableColumn id="3" name="10 - Fígado A" dataDxfId="37">
       <calculatedColumnFormula>Table1[[#This Row],[10 - Fígado A]]/Table1[[#This Row],[Rescale A_10]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="2 - Fígado B" dataDxfId="43">
+    <tableColumn id="7" name="2 - Fígado B" dataDxfId="36">
       <calculatedColumnFormula>Table1[[#This Row],[2 - Fígado B]]/Table1[[#This Row],[Rescale A_2]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="10 - Fígado B" dataDxfId="42">
+    <tableColumn id="8" name="10 - Fígado B" dataDxfId="35">
       <calculatedColumnFormula>Table1[[#This Row],[10 - Fígado B]]/Table1[[#This Row],[Rescale A_10]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="2 - Fígado C" dataDxfId="41">
+    <tableColumn id="9" name="2 - Fígado C" dataDxfId="34">
       <calculatedColumnFormula>Table1[[#This Row],[2 - Fígado C]]/Table1[[#This Row],[Rescale A_2]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="10 - Fígado C" dataDxfId="40">
+    <tableColumn id="10" name="10 - Fígado C" dataDxfId="33">
       <calculatedColumnFormula>Table1[[#This Row],[10 - Fígado C]]/Table1[[#This Row],[Rescale A_10]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="2 - Rim " dataDxfId="39">
+    <tableColumn id="11" name="2 - Rim " dataDxfId="32">
       <calculatedColumnFormula>Table1[[#This Row],[2 - Rim ]]/Table1[[#This Row],[Rescale A_2]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="10 - Rim" dataDxfId="38">
+    <tableColumn id="12" name="10 - Rim" dataDxfId="31">
       <calculatedColumnFormula>Table1[[#This Row],[10 - Rim]]/Table1[[#This Row],[Rescale A_10]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="2 - Gordura A" dataDxfId="37">
+    <tableColumn id="13" name="2 - Gordura A" dataDxfId="30">
       <calculatedColumnFormula>Table1[[#This Row],[2 - Gordura A]]/Table1[[#This Row],[Rescale A_2]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="10 - Gordura A" dataDxfId="36">
+    <tableColumn id="14" name="10 - Gordura A" dataDxfId="29">
       <calculatedColumnFormula>Table1[[#This Row],[10 - Gordura A]]/Table1[[#This Row],[Rescale A_10]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="2 - Gordura B" dataDxfId="35">
+    <tableColumn id="15" name="2 - Gordura B" dataDxfId="28">
       <calculatedColumnFormula>Table1[[#This Row],[2 - Gordura B]]/Table1[[#This Row],[Rescale A_2]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="10 - Gordura B" dataDxfId="34">
+    <tableColumn id="16" name="10 - Gordura B" dataDxfId="27">
       <calculatedColumnFormula>Table1[[#This Row],[10 - Gordura B]]/Table1[[#This Row],[Rescale A_10]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2010,21 +3603,21 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="P1:T23" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="P1:T23" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
   <tableColumns count="5">
-    <tableColumn id="1" name="A10 - Ideal (alpha)" dataDxfId="31">
+    <tableColumn id="1" name="A10 - Ideal (alpha)" dataDxfId="24">
       <calculatedColumnFormula>$B$25*Table43[[#This Row],[2 - Gordura A]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="A10 - 10ideal/10real (beta)" dataDxfId="30">
+    <tableColumn id="2" name="A10 - 10ideal/10real (beta)" dataDxfId="23">
       <calculatedColumnFormula>P2/Table43[[#This Row],[10 - Gordura A]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="B10 - Ideal (alpha)" dataDxfId="29">
+    <tableColumn id="3" name="B10 - Ideal (alpha)" dataDxfId="22">
       <calculatedColumnFormula>$B$25*Table43[[#This Row],[2 - Gordura B]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="B10 - 10ideal/10real (beta)" dataDxfId="28">
+    <tableColumn id="4" name="B10 - 10ideal/10real (beta)" dataDxfId="21">
       <calculatedColumnFormula>Table3[[#This Row],[B10 - Ideal (alpha)]]/Table43[[#This Row],[10 - Gordura B]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Avg Beta" dataDxfId="27">
+    <tableColumn id="5" name="Avg Beta" dataDxfId="20">
       <calculatedColumnFormula>AVERAGE(Table3[[#This Row],[B10 - 10ideal/10real (beta)]],Table3[[#This Row],[A10 - 10ideal/10real (beta)]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2033,25 +3626,25 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table610" displayName="Table610" ref="A2:G24" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table610" displayName="Table610" ref="A2:G24" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
   <tableColumns count="7">
-    <tableColumn id="1" name="Paciente" dataDxfId="24"/>
-    <tableColumn id="2" name="Fígado A" dataDxfId="23">
+    <tableColumn id="1" name="Paciente" dataDxfId="17"/>
+    <tableColumn id="2" name="Fígado A" dataDxfId="16">
       <calculatedColumnFormula>(Rescaled!C2-Rescaled!B2)/(Original!$B$26-Original!$B$25)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Fígado B" dataDxfId="22">
+    <tableColumn id="3" name="Fígado B" dataDxfId="15">
       <calculatedColumnFormula>(Rescaled!E2-Rescaled!D2)/(Original!$B$26-Original!$B$25)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Fígado C" dataDxfId="21">
+    <tableColumn id="4" name="Fígado C" dataDxfId="14">
       <calculatedColumnFormula>(Rescaled!G2-Rescaled!F2)/(Original!$B$26-Original!$B$25)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Rim" dataDxfId="20">
+    <tableColumn id="5" name="Rim" dataDxfId="13">
       <calculatedColumnFormula>(Rescaled!I2-Rescaled!H2)/(Original!$B$26-Original!$B$25)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Gordura A" dataDxfId="19">
+    <tableColumn id="6" name="Gordura A" dataDxfId="12">
       <calculatedColumnFormula>(Rescaled!K2-Rescaled!J2)/(Original!$B$26-Original!$B$25)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Gordura B" dataDxfId="18">
+    <tableColumn id="7" name="Gordura B" dataDxfId="11">
       <calculatedColumnFormula>(Rescaled!M2-Rescaled!L2)/(Original!$B$26-Original!$B$25)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2344,10 +3937,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q26"/>
+  <dimension ref="A1:X26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="X4" sqref="X4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2372,7 +3965,7 @@
     <col min="18" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:24">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2425,7 +4018,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:24">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -2477,8 +4070,25 @@
       <c r="Q2" s="3">
         <v>59.42</v>
       </c>
-    </row>
-    <row r="3" spans="1:17">
+      <c r="T2" s="4">
+        <v>1</v>
+      </c>
+      <c r="U2" s="4">
+        <f>$X$2*T2</f>
+        <v>2</v>
+      </c>
+      <c r="V2" s="4">
+        <f>$X$3*T2</f>
+        <v>3</v>
+      </c>
+      <c r="W2" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="X2" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -2530,8 +4140,25 @@
       <c r="Q3" s="3">
         <v>65.09</v>
       </c>
-    </row>
-    <row r="4" spans="1:17">
+      <c r="T3" s="4">
+        <v>10</v>
+      </c>
+      <c r="U3" s="4">
+        <f t="shared" ref="U3:U23" si="0">$X$2*T3</f>
+        <v>20</v>
+      </c>
+      <c r="V3" s="4">
+        <f t="shared" ref="V3:V18" si="1">$X$3*T3</f>
+        <v>30</v>
+      </c>
+      <c r="W3" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="X3" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -2583,8 +4210,19 @@
       <c r="Q4" s="3">
         <v>48.01</v>
       </c>
-    </row>
-    <row r="5" spans="1:17">
+      <c r="T4" s="4">
+        <v>20</v>
+      </c>
+      <c r="U4" s="4">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="V4" s="4">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -2636,8 +4274,19 @@
       <c r="Q5" s="3">
         <v>61.88</v>
       </c>
-    </row>
-    <row r="6" spans="1:17">
+      <c r="T5" s="4">
+        <v>30</v>
+      </c>
+      <c r="U5" s="4">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="V5" s="4">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -2689,8 +4338,19 @@
       <c r="Q6" s="3">
         <v>45.79</v>
       </c>
-    </row>
-    <row r="7" spans="1:17">
+      <c r="T6" s="4">
+        <v>40</v>
+      </c>
+      <c r="U6" s="4">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="V6" s="4">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -2742,8 +4402,19 @@
       <c r="Q7" s="3">
         <v>80.069999999999993</v>
       </c>
-    </row>
-    <row r="8" spans="1:17">
+      <c r="T7" s="4">
+        <v>50</v>
+      </c>
+      <c r="U7" s="4">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="V7" s="4">
+        <f t="shared" si="1"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -2795,8 +4466,19 @@
       <c r="Q8" s="3">
         <v>56.12</v>
       </c>
-    </row>
-    <row r="9" spans="1:17">
+      <c r="T8" s="4">
+        <v>60</v>
+      </c>
+      <c r="U8" s="4">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="V8" s="4">
+        <f t="shared" si="1"/>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -2848,8 +4530,19 @@
       <c r="Q9" s="3">
         <v>63.32</v>
       </c>
-    </row>
-    <row r="10" spans="1:17">
+      <c r="T9" s="4">
+        <v>70</v>
+      </c>
+      <c r="U9" s="4">
+        <f t="shared" si="0"/>
+        <v>140</v>
+      </c>
+      <c r="V9" s="4">
+        <f t="shared" si="1"/>
+        <v>210</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -2901,8 +4594,19 @@
       <c r="Q10" s="3">
         <v>83.56</v>
       </c>
-    </row>
-    <row r="11" spans="1:17">
+      <c r="T10" s="4">
+        <v>80</v>
+      </c>
+      <c r="U10" s="4">
+        <f t="shared" si="0"/>
+        <v>160</v>
+      </c>
+      <c r="V10" s="4">
+        <f t="shared" si="1"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -2954,8 +4658,19 @@
       <c r="Q11" s="3">
         <v>53.91</v>
       </c>
-    </row>
-    <row r="12" spans="1:17">
+      <c r="T11" s="4">
+        <v>90</v>
+      </c>
+      <c r="U11" s="4">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="V11" s="4">
+        <f t="shared" si="1"/>
+        <v>270</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -3007,8 +4722,19 @@
       <c r="Q12" s="3">
         <v>71.19</v>
       </c>
-    </row>
-    <row r="13" spans="1:17">
+      <c r="T12" s="4">
+        <v>100</v>
+      </c>
+      <c r="U12" s="4">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="V12" s="4">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
@@ -3060,8 +4786,19 @@
       <c r="Q13" s="3">
         <v>69.2</v>
       </c>
-    </row>
-    <row r="14" spans="1:17">
+      <c r="T13" s="4">
+        <v>110</v>
+      </c>
+      <c r="U13" s="4">
+        <f t="shared" si="0"/>
+        <v>220</v>
+      </c>
+      <c r="V13" s="4">
+        <f t="shared" si="1"/>
+        <v>330</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -3113,8 +4850,19 @@
       <c r="Q14" s="3">
         <v>55.6</v>
       </c>
-    </row>
-    <row r="15" spans="1:17">
+      <c r="T14" s="4">
+        <v>120</v>
+      </c>
+      <c r="U14" s="4">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+      <c r="V14" s="4">
+        <f t="shared" si="1"/>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
@@ -3166,8 +4914,19 @@
       <c r="Q15" s="3">
         <v>68.099999999999994</v>
       </c>
-    </row>
-    <row r="16" spans="1:17">
+      <c r="T15" s="4">
+        <v>130</v>
+      </c>
+      <c r="U15" s="4">
+        <f t="shared" si="0"/>
+        <v>260</v>
+      </c>
+      <c r="V15" s="4">
+        <f t="shared" si="1"/>
+        <v>390</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
@@ -3219,8 +4978,19 @@
       <c r="Q16" s="3">
         <v>68.41</v>
       </c>
-    </row>
-    <row r="17" spans="1:17">
+      <c r="T16" s="4">
+        <v>140</v>
+      </c>
+      <c r="U16" s="4">
+        <f t="shared" si="0"/>
+        <v>280</v>
+      </c>
+      <c r="V16" s="4">
+        <f t="shared" si="1"/>
+        <v>420</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
@@ -3272,8 +5042,19 @@
       <c r="Q17" s="3">
         <v>56.74</v>
       </c>
-    </row>
-    <row r="18" spans="1:17">
+      <c r="T17" s="4">
+        <v>150</v>
+      </c>
+      <c r="U17" s="4">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+      <c r="V17" s="4">
+        <f t="shared" si="1"/>
+        <v>450</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
@@ -3325,8 +5106,19 @@
       <c r="Q18" s="3">
         <v>49.36</v>
       </c>
-    </row>
-    <row r="19" spans="1:17">
+      <c r="T18" s="4">
+        <v>160</v>
+      </c>
+      <c r="U18" s="4">
+        <f t="shared" si="0"/>
+        <v>320</v>
+      </c>
+      <c r="V18" s="4">
+        <f t="shared" si="1"/>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22">
       <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
@@ -3379,7 +5171,7 @@
         <v>68.17</v>
       </c>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:22">
       <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
@@ -3432,7 +5224,7 @@
         <v>76.25</v>
       </c>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:22">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
@@ -3485,7 +5277,7 @@
         <v>52.39</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:22">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
@@ -3538,7 +5330,7 @@
         <v>99.85</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:22">
       <c r="A23" s="3" t="s">
         <v>22</v>
       </c>
@@ -3591,7 +5383,7 @@
         <v>61.49</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:22">
       <c r="A25" s="3" t="s">
         <v>45</v>
       </c>
@@ -3599,7 +5391,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="1:22">
       <c r="A26" s="3" t="s">
         <v>46</v>
       </c>
@@ -3610,18 +5402,19 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M23"/>
+  <dimension ref="A1:Z51"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" topLeftCell="E19" workbookViewId="0">
+      <selection activeCell="P28" sqref="P28:S47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3639,10 +5432,15 @@
     <col min="11" max="11" width="18.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17" style="3" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="18.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="3"/>
+    <col min="14" max="15" width="9.140625" style="3"/>
+    <col min="16" max="16" width="7.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:20">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3683,7 +5481,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:20">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -3735,8 +5533,22 @@
         <f>Table1[[#This Row],[10 - Gordura B]]/Table1[[#This Row],[Rescale A_10]]</f>
         <v>11.650980392156864</v>
       </c>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="P2" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="4">
+        <f>$T$2*P2</f>
+        <v>4.74</v>
+      </c>
+      <c r="R2" s="4"/>
+      <c r="S2" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="T2" s="15">
+        <v>4.74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -3788,8 +5600,18 @@
         <f>Table1[[#This Row],[10 - Gordura B]]/Table1[[#This Row],[Rescale A_10]]</f>
         <v>12.281132075471699</v>
       </c>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="P3" s="4">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="4">
+        <f t="shared" ref="Q3:Q23" si="0">$T$2*P3</f>
+        <v>9.48</v>
+      </c>
+      <c r="R3" s="4"/>
+      <c r="S3" s="4"/>
+      <c r="T3" s="4"/>
+    </row>
+    <row r="4" spans="1:20">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -3841,8 +5663,18 @@
         <f>Table1[[#This Row],[10 - Gordura B]]/Table1[[#This Row],[Rescale A_10]]</f>
         <v>9.679435483870968</v>
       </c>
-    </row>
-    <row r="5" spans="1:13">
+      <c r="P4" s="4">
+        <v>3</v>
+      </c>
+      <c r="Q4" s="4">
+        <f t="shared" si="0"/>
+        <v>14.22</v>
+      </c>
+      <c r="R4" s="4"/>
+      <c r="S4" s="4"/>
+      <c r="T4" s="4"/>
+    </row>
+    <row r="5" spans="1:20">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -3894,8 +5726,18 @@
         <f>Table1[[#This Row],[10 - Gordura B]]/Table1[[#This Row],[Rescale A_10]]</f>
         <v>10.382550335570471</v>
       </c>
-    </row>
-    <row r="6" spans="1:13">
+      <c r="P5" s="4">
+        <v>4</v>
+      </c>
+      <c r="Q5" s="4">
+        <f t="shared" si="0"/>
+        <v>18.96</v>
+      </c>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+    </row>
+    <row r="6" spans="1:20">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -3947,8 +5789,18 @@
         <f>Table1[[#This Row],[10 - Gordura B]]/Table1[[#This Row],[Rescale A_10]]</f>
         <v>9.6197478991596643</v>
       </c>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="P6" s="4">
+        <v>5</v>
+      </c>
+      <c r="Q6" s="4">
+        <f t="shared" si="0"/>
+        <v>23.700000000000003</v>
+      </c>
+      <c r="R6" s="4"/>
+      <c r="S6" s="4"/>
+      <c r="T6" s="4"/>
+    </row>
+    <row r="7" spans="1:20">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -4000,8 +5852,18 @@
         <f>Table1[[#This Row],[10 - Gordura B]]/Table1[[#This Row],[Rescale A_10]]</f>
         <v>18.449308755760367</v>
       </c>
-    </row>
-    <row r="8" spans="1:13">
+      <c r="P7" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q7" s="4">
+        <f t="shared" si="0"/>
+        <v>28.44</v>
+      </c>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+    </row>
+    <row r="8" spans="1:20">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -4053,8 +5915,18 @@
         <f>Table1[[#This Row],[10 - Gordura B]]/Table1[[#This Row],[Rescale A_10]]</f>
         <v>9.76</v>
       </c>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="P8" s="4">
+        <v>7</v>
+      </c>
+      <c r="Q8" s="4">
+        <f t="shared" si="0"/>
+        <v>33.18</v>
+      </c>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
+    </row>
+    <row r="9" spans="1:20">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -4106,8 +5978,18 @@
         <f>Table1[[#This Row],[10 - Gordura B]]/Table1[[#This Row],[Rescale A_10]]</f>
         <v>12.740442655935615</v>
       </c>
-    </row>
-    <row r="10" spans="1:13">
+      <c r="P9" s="4">
+        <v>8</v>
+      </c>
+      <c r="Q9" s="4">
+        <f t="shared" si="0"/>
+        <v>37.92</v>
+      </c>
+      <c r="R9" s="4"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+    </row>
+    <row r="10" spans="1:20">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -4159,8 +6041,18 @@
         <f>Table1[[#This Row],[10 - Gordura B]]/Table1[[#This Row],[Rescale A_10]]</f>
         <v>22.402144772117964</v>
       </c>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="P10" s="4">
+        <v>9</v>
+      </c>
+      <c r="Q10" s="4">
+        <f t="shared" si="0"/>
+        <v>42.660000000000004</v>
+      </c>
+      <c r="R10" s="4"/>
+      <c r="S10" s="4"/>
+      <c r="T10" s="4"/>
+    </row>
+    <row r="11" spans="1:20">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -4212,8 +6104,18 @@
         <f>Table1[[#This Row],[10 - Gordura B]]/Table1[[#This Row],[Rescale A_10]]</f>
         <v>9.8736263736263723</v>
       </c>
-    </row>
-    <row r="12" spans="1:13">
+      <c r="P11" s="4">
+        <v>10</v>
+      </c>
+      <c r="Q11" s="4">
+        <f t="shared" si="0"/>
+        <v>47.400000000000006</v>
+      </c>
+      <c r="R11" s="4"/>
+      <c r="S11" s="4"/>
+      <c r="T11" s="4"/>
+    </row>
+    <row r="12" spans="1:20">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -4265,8 +6167,18 @@
         <f>Table1[[#This Row],[10 - Gordura B]]/Table1[[#This Row],[Rescale A_10]]</f>
         <v>27.171755725190838</v>
       </c>
-    </row>
-    <row r="13" spans="1:13">
+      <c r="P12" s="4">
+        <v>11</v>
+      </c>
+      <c r="Q12" s="4">
+        <f t="shared" si="0"/>
+        <v>52.14</v>
+      </c>
+      <c r="R12" s="4"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="4"/>
+    </row>
+    <row r="13" spans="1:20">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
@@ -4318,8 +6230,18 @@
         <f>Table1[[#This Row],[10 - Gordura B]]/Table1[[#This Row],[Rescale A_10]]</f>
         <v>14.122448979591836</v>
       </c>
-    </row>
-    <row r="14" spans="1:13">
+      <c r="P13" s="4">
+        <v>12</v>
+      </c>
+      <c r="Q13" s="4">
+        <f t="shared" si="0"/>
+        <v>56.88</v>
+      </c>
+      <c r="R13" s="4"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="4"/>
+    </row>
+    <row r="14" spans="1:20">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -4371,8 +6293,18 @@
         <f>Table1[[#This Row],[10 - Gordura B]]/Table1[[#This Row],[Rescale A_10]]</f>
         <v>13.238095238095237</v>
       </c>
-    </row>
-    <row r="15" spans="1:13">
+      <c r="P14" s="4">
+        <v>14</v>
+      </c>
+      <c r="Q14" s="4">
+        <f t="shared" si="0"/>
+        <v>66.36</v>
+      </c>
+      <c r="R14" s="4"/>
+      <c r="S14" s="4"/>
+      <c r="T14" s="4"/>
+    </row>
+    <row r="15" spans="1:20">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
@@ -4424,8 +6356,18 @@
         <f>Table1[[#This Row],[10 - Gordura B]]/Table1[[#This Row],[Rescale A_10]]</f>
         <v>13.249027237354085</v>
       </c>
-    </row>
-    <row r="16" spans="1:13">
+      <c r="P15" s="4">
+        <v>15</v>
+      </c>
+      <c r="Q15" s="4">
+        <f t="shared" si="0"/>
+        <v>71.100000000000009</v>
+      </c>
+      <c r="R15" s="4"/>
+      <c r="S15" s="4"/>
+      <c r="T15" s="4"/>
+    </row>
+    <row r="16" spans="1:20">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
@@ -4477,8 +6419,18 @@
         <f>Table1[[#This Row],[10 - Gordura B]]/Table1[[#This Row],[Rescale A_10]]</f>
         <v>11.575296108291031</v>
       </c>
-    </row>
-    <row r="17" spans="1:13">
+      <c r="P16" s="4">
+        <v>16</v>
+      </c>
+      <c r="Q16" s="4">
+        <f t="shared" si="0"/>
+        <v>75.84</v>
+      </c>
+      <c r="R16" s="4"/>
+      <c r="S16" s="4"/>
+      <c r="T16" s="4"/>
+    </row>
+    <row r="17" spans="1:26">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
@@ -4530,8 +6482,18 @@
         <f>Table1[[#This Row],[10 - Gordura B]]/Table1[[#This Row],[Rescale A_10]]</f>
         <v>9.633276740237692</v>
       </c>
-    </row>
-    <row r="18" spans="1:13">
+      <c r="P17" s="4">
+        <v>17</v>
+      </c>
+      <c r="Q17" s="4">
+        <f t="shared" si="0"/>
+        <v>80.58</v>
+      </c>
+      <c r="R17" s="4"/>
+      <c r="S17" s="4"/>
+      <c r="T17" s="4"/>
+    </row>
+    <row r="18" spans="1:26">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
@@ -4583,8 +6545,18 @@
         <f>Table1[[#This Row],[10 - Gordura B]]/Table1[[#This Row],[Rescale A_10]]</f>
         <v>6.7156462585034014</v>
       </c>
-    </row>
-    <row r="19" spans="1:13">
+      <c r="P18" s="4">
+        <v>18</v>
+      </c>
+      <c r="Q18" s="4">
+        <f t="shared" si="0"/>
+        <v>85.320000000000007</v>
+      </c>
+      <c r="R18" s="4"/>
+      <c r="S18" s="4"/>
+      <c r="T18" s="4"/>
+    </row>
+    <row r="19" spans="1:26">
       <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
@@ -4636,8 +6608,18 @@
         <f>Table1[[#This Row],[10 - Gordura B]]/Table1[[#This Row],[Rescale A_10]]</f>
         <v>34.429292929292927</v>
       </c>
-    </row>
-    <row r="20" spans="1:13">
+      <c r="P19" s="4">
+        <v>19</v>
+      </c>
+      <c r="Q19" s="4">
+        <f t="shared" si="0"/>
+        <v>90.06</v>
+      </c>
+      <c r="R19" s="4"/>
+      <c r="S19" s="4"/>
+      <c r="T19" s="4"/>
+    </row>
+    <row r="20" spans="1:26">
       <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
@@ -4689,8 +6671,18 @@
         <f>Table1[[#This Row],[10 - Gordura B]]/Table1[[#This Row],[Rescale A_10]]</f>
         <v>15.754132231404959</v>
       </c>
-    </row>
-    <row r="21" spans="1:13">
+      <c r="P20" s="4">
+        <v>20</v>
+      </c>
+      <c r="Q20" s="4">
+        <f t="shared" si="0"/>
+        <v>94.800000000000011</v>
+      </c>
+      <c r="R20" s="4"/>
+      <c r="S20" s="4"/>
+      <c r="T20" s="4"/>
+    </row>
+    <row r="21" spans="1:26">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
@@ -4742,8 +6734,13 @@
         <f>Table1[[#This Row],[10 - Gordura B]]/Table1[[#This Row],[Rescale A_10]]</f>
         <v>8.2503937007874022</v>
       </c>
-    </row>
-    <row r="22" spans="1:13">
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4"/>
+      <c r="R21" s="4"/>
+      <c r="S21" s="4"/>
+      <c r="T21" s="4"/>
+    </row>
+    <row r="22" spans="1:26">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
@@ -4795,8 +6792,13 @@
         <f>Table1[[#This Row],[10 - Gordura B]]/Table1[[#This Row],[Rescale A_10]]</f>
         <v>29.110787172011658</v>
       </c>
-    </row>
-    <row r="23" spans="1:13">
+      <c r="P22" s="4"/>
+      <c r="Q22" s="4"/>
+      <c r="R22" s="4"/>
+      <c r="S22" s="4"/>
+      <c r="T22" s="4"/>
+    </row>
+    <row r="23" spans="1:26">
       <c r="A23" s="3" t="s">
         <v>22</v>
       </c>
@@ -4848,12 +6850,864 @@
         <f>Table1[[#This Row],[10 - Gordura B]]/Table1[[#This Row],[Rescale A_10]]</f>
         <v>10.40439932318105</v>
       </c>
+      <c r="P23" s="4"/>
+      <c r="Q23" s="4"/>
+      <c r="R23" s="4"/>
+      <c r="S23" s="4"/>
+      <c r="T23" s="4"/>
+    </row>
+    <row r="26" spans="1:26">
+      <c r="K26" s="3">
+        <v>2</v>
+      </c>
+      <c r="L26" s="3">
+        <v>10</v>
+      </c>
+      <c r="M26" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="N26" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="P26" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q26" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="R26" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="S26" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="X26" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y26" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="Z26" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26">
+      <c r="K27" s="6">
+        <v>3.275167785234899</v>
+      </c>
+      <c r="L27" s="6">
+        <v>37.717647058823538</v>
+      </c>
+      <c r="X27" s="3">
+        <v>2</v>
+      </c>
+      <c r="Y27" s="3">
+        <f>SIN(X27*PI()/180)</f>
+        <v>3.4899496702500969E-2</v>
+      </c>
+      <c r="Z27" s="3">
+        <f>COS(X27*PI()/180)</f>
+        <v>0.99939082701909576</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26">
+      <c r="K28" s="6">
+        <v>11.490523968784837</v>
+      </c>
+      <c r="L28" s="6">
+        <v>49.698113207547166</v>
+      </c>
+      <c r="M28" s="3">
+        <f t="shared" ref="M28:M47" si="1">K28/K28</f>
+        <v>1</v>
+      </c>
+      <c r="N28" s="3">
+        <f t="shared" ref="N28:N47" si="2">L28/K28</f>
+        <v>4.3251389877917736</v>
+      </c>
+      <c r="P28" s="16">
+        <f>K28*$Y$28/(L28*$Y$27)</f>
+        <v>1.1504056290554365</v>
+      </c>
+      <c r="Q28" s="16">
+        <f>-$Y$30/LN((P28-1)/(P28*$Z$27-$Z$28))</f>
+        <v>1.7611436189939376</v>
+      </c>
+      <c r="R28" s="16">
+        <f>M28*$Y$28/(N28*$Y$27)</f>
+        <v>1.1504056290554363</v>
+      </c>
+      <c r="S28" s="16">
+        <f>-$Y$30/LN((R28-1)/(R28*$Z$27-$Z$28))</f>
+        <v>1.7611436189939353</v>
+      </c>
+      <c r="U28" s="3">
+        <v>1.7611436189939329</v>
+      </c>
+      <c r="W28" s="3">
+        <f>M28-0.2</f>
+        <v>0.8</v>
+      </c>
+      <c r="X28" s="3">
+        <v>10</v>
+      </c>
+      <c r="Y28" s="3">
+        <f>SIN(X28*PI()/180)</f>
+        <v>0.17364817766693033</v>
+      </c>
+      <c r="Z28" s="3">
+        <f>COS(X28*PI()/180)</f>
+        <v>0.98480775301220802</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26">
+      <c r="K29" s="6">
+        <v>8.8557347670250888</v>
+      </c>
+      <c r="L29" s="6">
+        <v>41.8125</v>
+      </c>
+      <c r="M29" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N29" s="3">
+        <f t="shared" si="2"/>
+        <v>4.7215167459273504</v>
+      </c>
+      <c r="P29" s="16">
+        <f>K29*$Y$28/(L29*$Y$27)</f>
+        <v>1.0538275104699477</v>
+      </c>
+      <c r="Q29" s="16">
+        <f>-$Y$30/LN((P29-1)/(P29*$Z$27-$Z$28))</f>
+        <v>0.67707794546015254</v>
+      </c>
+      <c r="R29" s="16">
+        <f>M29*$Y$28/(N29*$Y$27)</f>
+        <v>1.0538275104699477</v>
+      </c>
+      <c r="S29" s="16">
+        <f>-$Y$30/LN((R29-1)/(R29*$Z$27-$Z$28))</f>
+        <v>0.67707794546015254</v>
+      </c>
+      <c r="U29" s="3">
+        <v>0.67707794546015576</v>
+      </c>
+      <c r="W29" s="3">
+        <f>M29-0.2</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26">
+      <c r="K30" s="6">
+        <v>9.6373626373626369</v>
+      </c>
+      <c r="L30" s="6">
+        <v>42.510067114093964</v>
+      </c>
+      <c r="M30" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N30" s="3">
+        <f t="shared" si="2"/>
+        <v>4.4109647746665344</v>
+      </c>
+      <c r="P30" s="16">
+        <f>K30*$Y$28/(L30*$Y$27)</f>
+        <v>1.1280217576389384</v>
+      </c>
+      <c r="Q30" s="16">
+        <f>-$Y$30/LN((P30-1)/(P30*$Z$27-$Z$28))</f>
+        <v>1.5093617935882717</v>
+      </c>
+      <c r="R30" s="16">
+        <f>M30*$Y$28/(N30*$Y$27)</f>
+        <v>1.1280217576389386</v>
+      </c>
+      <c r="S30" s="16">
+        <f>-$Y$30/LN((R30-1)/(R30*$Z$27-$Z$28))</f>
+        <v>1.5093617935882735</v>
+      </c>
+      <c r="U30" s="3">
+        <v>1.5093617935882702</v>
+      </c>
+      <c r="W30" s="3">
+        <f>M30-0.2</f>
+        <v>0.8</v>
+      </c>
+      <c r="X30" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y30" s="3">
+        <v>0.16200000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26">
+      <c r="K31" s="6">
+        <v>7.3270440251572317</v>
+      </c>
+      <c r="L31" s="6">
+        <v>35.338235294117652</v>
+      </c>
+      <c r="M31" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N31" s="3">
+        <f t="shared" si="2"/>
+        <v>4.8229866195405213</v>
+      </c>
+      <c r="P31" s="16">
+        <f>K31*$Y$28/(L31*$Y$27)</f>
+        <v>1.0316562392778965</v>
+      </c>
+      <c r="Q31" s="16">
+        <f>-$Y$30/LN((P31-1)/(P31*$Z$27-$Z$28))</f>
+        <v>0.4280301934750958</v>
+      </c>
+      <c r="R31" s="16">
+        <f>M31*$Y$28/(N31*$Y$27)</f>
+        <v>1.0316562392778965</v>
+      </c>
+      <c r="S31" s="16">
+        <f>-$Y$30/LN((R31-1)/(R31*$Z$27-$Z$28))</f>
+        <v>0.4280301934750958</v>
+      </c>
+      <c r="U31" s="3">
+        <v>0.42803019347509341</v>
+      </c>
+      <c r="W31" s="3">
+        <f>M31-0.2</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26">
+      <c r="K32" s="6">
+        <v>20.40360610263523</v>
+      </c>
+      <c r="L32" s="6">
+        <v>67.559907834101381</v>
+      </c>
+      <c r="M32" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N32" s="3">
+        <f t="shared" si="2"/>
+        <v>3.311174872434715</v>
+      </c>
+      <c r="P32" s="16">
+        <f>K32*$Y$28/(L32*$Y$27)</f>
+        <v>1.5026884503820153</v>
+      </c>
+      <c r="Q32" s="16">
+        <f>-$Y$30/LN((P32-1)/(P32*$Z$27-$Z$28))</f>
+        <v>5.7846483968471025</v>
+      </c>
+      <c r="R32" s="16">
+        <f>M32*$Y$28/(N32*$Y$27)</f>
+        <v>1.5026884503820153</v>
+      </c>
+      <c r="S32" s="16">
+        <f>-$Y$30/LN((R32-1)/(R32*$Z$27-$Z$28))</f>
+        <v>5.7846483968471025</v>
+      </c>
+      <c r="U32" s="3">
+        <v>5.7846483968471736</v>
+      </c>
+      <c r="W32" s="3">
+        <f>M32-0.2</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="33" spans="11:25">
+      <c r="K33" s="6">
+        <v>12.710858585858587</v>
+      </c>
+      <c r="L33" s="6">
+        <v>34.845217391304352</v>
+      </c>
+      <c r="M33" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N33" s="3">
+        <f t="shared" si="2"/>
+        <v>2.7413740115141598</v>
+      </c>
+      <c r="P33" s="16">
+        <f>K33*$Y$28/(L33*$Y$27)</f>
+        <v>1.8150256831443989</v>
+      </c>
+      <c r="Q33" s="16">
+        <f>-$Y$30/LN((P33-1)/(P33*$Z$27-$Z$28))</f>
+        <v>9.4538129635987005</v>
+      </c>
+      <c r="R33" s="16">
+        <f>M33*$Y$28/(N33*$Y$27)</f>
+        <v>1.8150256831443987</v>
+      </c>
+      <c r="S33" s="16">
+        <f>-$Y$30/LN((R33-1)/(R33*$Z$27-$Z$28))</f>
+        <v>9.4538129635987005</v>
+      </c>
+      <c r="U33" s="3">
+        <v>9.4538129635988248</v>
+      </c>
+      <c r="W33" s="3">
+        <f>M33-0.2</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="34" spans="11:25">
+      <c r="K34" s="6">
+        <v>10.810256410256411</v>
+      </c>
+      <c r="L34" s="6">
+        <v>46.91348088531187</v>
+      </c>
+      <c r="M34" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N34" s="3">
+        <f t="shared" si="2"/>
+        <v>4.3397195316109176</v>
+      </c>
+      <c r="P34" s="16">
+        <f>K34*$Y$28/(L34*$Y$27)</f>
+        <v>1.1465405083806894</v>
+      </c>
+      <c r="Q34" s="16">
+        <f>-$Y$30/LN((P34-1)/(P34*$Z$27-$Z$28))</f>
+        <v>1.7176378536963226</v>
+      </c>
+      <c r="R34" s="16">
+        <f>M34*$Y$28/(N34*$Y$27)</f>
+        <v>1.1465405083806894</v>
+      </c>
+      <c r="S34" s="16">
+        <f>-$Y$30/LN((R34-1)/(R34*$Z$27-$Z$28))</f>
+        <v>1.7176378536963226</v>
+      </c>
+      <c r="U34" s="3">
+        <v>1.7176378536963004</v>
+      </c>
+      <c r="W34" s="3">
+        <f>M34-0.2</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="35" spans="11:25">
+      <c r="K35" s="6">
+        <v>17.67715458276334</v>
+      </c>
+      <c r="L35" s="6">
+        <v>79.766756032171571</v>
+      </c>
+      <c r="M35" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N35" s="3">
+        <f t="shared" si="2"/>
+        <v>4.5124205741771721</v>
+      </c>
+      <c r="P35" s="16">
+        <f>K35*$Y$28/(L35*$Y$27)</f>
+        <v>1.1026596825829094</v>
+      </c>
+      <c r="Q35" s="16">
+        <f>-$Y$30/LN((P35-1)/(P35*$Z$27-$Z$28))</f>
+        <v>1.2245488615868059</v>
+      </c>
+      <c r="R35" s="16">
+        <f>M35*$Y$28/(N35*$Y$27)</f>
+        <v>1.1026596825829091</v>
+      </c>
+      <c r="S35" s="16">
+        <f>-$Y$30/LN((R35-1)/(R35*$Z$27-$Z$28))</f>
+        <v>1.2245488615868034</v>
+      </c>
+      <c r="U35" s="3">
+        <v>1.2245488615868163</v>
+      </c>
+      <c r="W35" s="3">
+        <f>M35-0.2</f>
+        <v>0.8</v>
+      </c>
+      <c r="X35" s="3">
+        <f>Y28/Y27</f>
+        <v>4.9756642380027891</v>
+      </c>
+      <c r="Y35" s="3">
+        <f>X35/T2</f>
+        <v>1.0497181936714743</v>
+      </c>
+    </row>
+    <row r="36" spans="11:25">
+      <c r="K36" s="6">
+        <v>12.864197530864198</v>
+      </c>
+      <c r="L36" s="6">
+        <v>45.998168498168496</v>
+      </c>
+      <c r="M36" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N36" s="3">
+        <f t="shared" si="2"/>
+        <v>3.5756733669401615</v>
+      </c>
+      <c r="P36" s="16">
+        <f>K36*$Y$28/(L36*$Y$27)</f>
+        <v>1.3915320912717071</v>
+      </c>
+      <c r="Q36" s="16">
+        <f>-$Y$30/LN((P36-1)/(P36*$Z$27-$Z$28))</f>
+        <v>4.5022730604685011</v>
+      </c>
+      <c r="R36" s="16">
+        <f>M36*$Y$28/(N36*$Y$27)</f>
+        <v>1.3915320912717071</v>
+      </c>
+      <c r="S36" s="16">
+        <f>-$Y$30/LN((R36-1)/(R36*$Z$27-$Z$28))</f>
+        <v>4.5022730604685011</v>
+      </c>
+      <c r="U36" s="3">
+        <v>4.5022730604685153</v>
+      </c>
+      <c r="W36" s="3">
+        <f>M36-0.2</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="37" spans="11:25">
+      <c r="K37" s="6">
+        <v>14.998908296943229</v>
+      </c>
+      <c r="L37" s="6">
+        <v>105.25954198473281</v>
+      </c>
+      <c r="P37" s="16"/>
+      <c r="Q37" s="16"/>
+      <c r="R37" s="16"/>
+      <c r="S37" s="16"/>
+    </row>
+    <row r="38" spans="11:25">
+      <c r="K38" s="6">
+        <v>10.258220502901354</v>
+      </c>
+      <c r="L38" s="6">
+        <v>43.316326530612244</v>
+      </c>
+      <c r="M38" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N38" s="3">
+        <f t="shared" si="2"/>
+        <v>4.2225965525269222</v>
+      </c>
+      <c r="P38" s="16">
+        <f>K38*$Y$28/(L38*$Y$27)</f>
+        <v>1.1783423247066334</v>
+      </c>
+      <c r="Q38" s="16">
+        <f>-$Y$30/LN((P38-1)/(P38*$Z$27-$Z$28))</f>
+        <v>2.0759804104281954</v>
+      </c>
+      <c r="R38" s="16">
+        <f>M38*$Y$28/(N38*$Y$27)</f>
+        <v>1.1783423247066334</v>
+      </c>
+      <c r="S38" s="16">
+        <f>-$Y$30/LN((R38-1)/(R38*$Z$27-$Z$28))</f>
+        <v>2.0759804104281954</v>
+      </c>
+      <c r="U38" s="3">
+        <v>2.0759804104282051</v>
+      </c>
+      <c r="W38" s="3">
+        <f>M38-0.2</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="39" spans="11:25">
+      <c r="K39" s="6">
+        <v>13.138443935926773</v>
+      </c>
+      <c r="L39" s="6">
+        <v>60.157142857142851</v>
+      </c>
+      <c r="M39" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N39" s="3">
+        <f t="shared" si="2"/>
+        <v>4.5787113870193199</v>
+      </c>
+      <c r="P39" s="16">
+        <f>K39*$Y$28/(L39*$Y$27)</f>
+        <v>1.0866953204582479</v>
+      </c>
+      <c r="Q39" s="16">
+        <f>-$Y$30/LN((P39-1)/(P39*$Z$27-$Z$28))</f>
+        <v>1.045487730213289</v>
+      </c>
+      <c r="R39" s="16">
+        <f>M39*$Y$28/(N39*$Y$27)</f>
+        <v>1.0866953204582481</v>
+      </c>
+      <c r="S39" s="16">
+        <f>-$Y$30/LN((R39-1)/(R39*$Z$27-$Z$28))</f>
+        <v>1.0454877302132917</v>
+      </c>
+      <c r="U39" s="3">
+        <v>1.0454877302133012</v>
+      </c>
+      <c r="W39" s="3">
+        <f>M39-0.2</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="40" spans="11:25">
+      <c r="K40" s="6">
+        <v>12.319514661274013</v>
+      </c>
+      <c r="L40" s="6">
+        <v>55.175097276264601</v>
+      </c>
+      <c r="M40" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N40" s="3">
+        <f t="shared" si="2"/>
+        <v>4.4786745901367118</v>
+      </c>
+      <c r="P40" s="16">
+        <f>K40*$Y$28/(L40*$Y$27)</f>
+        <v>1.1109680191904514</v>
+      </c>
+      <c r="Q40" s="16">
+        <f>-$Y$30/LN((P40-1)/(P40*$Z$27-$Z$28))</f>
+        <v>1.3177997023817716</v>
+      </c>
+      <c r="R40" s="16">
+        <f>M40*$Y$28/(N40*$Y$27)</f>
+        <v>1.1109680191904514</v>
+      </c>
+      <c r="S40" s="16">
+        <f>-$Y$30/LN((R40-1)/(R40*$Z$27-$Z$28))</f>
+        <v>1.3177997023817716</v>
+      </c>
+      <c r="U40" s="3">
+        <v>1.3177997023817838</v>
+      </c>
+      <c r="W40" s="3">
+        <f>M40-0.2</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="41" spans="11:25">
+      <c r="K41" s="6">
+        <v>7.9821092278719403</v>
+      </c>
+      <c r="L41" s="6">
+        <v>31.387478849407781</v>
+      </c>
+      <c r="M41" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N41" s="3">
+        <f t="shared" si="2"/>
+        <v>3.9322286820893075</v>
+      </c>
+      <c r="P41" s="16">
+        <f>K41*$Y$28/(L41*$Y$27)</f>
+        <v>1.2653547492459349</v>
+      </c>
+      <c r="Q41" s="16">
+        <f>-$Y$30/LN((P41-1)/(P41*$Z$27-$Z$28))</f>
+        <v>3.0610911009201853</v>
+      </c>
+      <c r="R41" s="16">
+        <f>M41*$Y$28/(N41*$Y$27)</f>
+        <v>1.2653547492459349</v>
+      </c>
+      <c r="S41" s="16">
+        <f>-$Y$30/LN((R41-1)/(R41*$Z$27-$Z$28))</f>
+        <v>3.0610911009201853</v>
+      </c>
+      <c r="U41" s="3">
+        <v>3.061091100920192</v>
+      </c>
+      <c r="W41" s="3">
+        <f>M41-0.2</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="42" spans="11:25">
+      <c r="K42" s="6">
+        <v>8.6000000000000014</v>
+      </c>
+      <c r="L42" s="6">
+        <v>32.173174872665534</v>
+      </c>
+      <c r="M42" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N42" s="3">
+        <f t="shared" si="2"/>
+        <v>3.7410668456587826</v>
+      </c>
+      <c r="P42" s="16">
+        <f>K42*$Y$28/(L42*$Y$27)</f>
+        <v>1.3300121177403341</v>
+      </c>
+      <c r="Q42" s="16">
+        <f>-$Y$30/LN((P42-1)/(P42*$Z$27-$Z$28))</f>
+        <v>3.7976968502088377</v>
+      </c>
+      <c r="R42" s="16">
+        <f>M42*$Y$28/(N42*$Y$27)</f>
+        <v>1.3300121177403341</v>
+      </c>
+      <c r="S42" s="16">
+        <f>-$Y$30/LN((R42-1)/(R42*$Z$27-$Z$28))</f>
+        <v>3.7976968502088377</v>
+      </c>
+      <c r="U42" s="3">
+        <v>3.7976968502088173</v>
+      </c>
+      <c r="W42" s="3">
+        <f>M42-0.2</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="43" spans="11:25">
+      <c r="K43" s="6">
+        <v>6.0271828665568368</v>
+      </c>
+      <c r="L43" s="6">
+        <v>21.189115646258507</v>
+      </c>
+      <c r="M43" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N43" s="3">
+        <f t="shared" si="2"/>
+        <v>3.5155919631758685</v>
+      </c>
+      <c r="P43" s="16">
+        <f>K43*$Y$28/(L43*$Y$27)</f>
+        <v>1.4153133498200228</v>
+      </c>
+      <c r="Q43" s="16">
+        <f>-$Y$30/LN((P43-1)/(P43*$Z$27-$Z$28))</f>
+        <v>4.7756156281657471</v>
+      </c>
+      <c r="R43" s="16">
+        <f>M43*$Y$28/(N43*$Y$27)</f>
+        <v>1.4153133498200228</v>
+      </c>
+      <c r="S43" s="16">
+        <f>-$Y$30/LN((R43-1)/(R43*$Z$27-$Z$28))</f>
+        <v>4.7756156281657471</v>
+      </c>
+      <c r="U43" s="3">
+        <v>4.7756156281658271</v>
+      </c>
+      <c r="W43" s="3">
+        <f>M43-0.2</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="44" spans="11:25">
+      <c r="K44" s="6">
+        <v>16.101376720901126</v>
+      </c>
+      <c r="L44" s="6">
+        <v>51.16115702479339</v>
+      </c>
+      <c r="M44" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N44" s="3">
+        <f t="shared" si="2"/>
+        <v>3.1774399116059011</v>
+      </c>
+      <c r="P44" s="16">
+        <f>K44*$Y$28/(L44*$Y$27)</f>
+        <v>1.5659349590935463</v>
+      </c>
+      <c r="Q44" s="16">
+        <f>-$Y$30/LN((P44-1)/(P44*$Z$27-$Z$28))</f>
+        <v>6.519728458894841</v>
+      </c>
+      <c r="R44" s="16">
+        <f>M44*$Y$28/(N44*$Y$27)</f>
+        <v>1.5659349590935465</v>
+      </c>
+      <c r="S44" s="16">
+        <f>-$Y$30/LN((R44-1)/(R44*$Z$27-$Z$28))</f>
+        <v>6.519728458894841</v>
+      </c>
+      <c r="U44" s="3">
+        <v>6.5197284588949005</v>
+      </c>
+      <c r="W44" s="3">
+        <f>M44-0.2</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="45" spans="11:25">
+      <c r="K45" s="6">
+        <v>6.7399650959860375</v>
+      </c>
+      <c r="L45" s="6">
+        <v>27.604724409448821</v>
+      </c>
+      <c r="M45" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N45" s="3">
+        <f t="shared" si="2"/>
+        <v>4.0956776505992174</v>
+      </c>
+      <c r="P45" s="16">
+        <f>K45*$Y$28/(L45*$Y$27)</f>
+        <v>1.2148573844122781</v>
+      </c>
+      <c r="Q45" s="16">
+        <f>-$Y$30/LN((P45-1)/(P45*$Z$27-$Z$28))</f>
+        <v>2.488538187070489</v>
+      </c>
+      <c r="R45" s="16">
+        <f>M45*$Y$28/(N45*$Y$27)</f>
+        <v>1.2148573844122781</v>
+      </c>
+      <c r="S45" s="16">
+        <f>-$Y$30/LN((R45-1)/(R45*$Z$27-$Z$28))</f>
+        <v>2.488538187070489</v>
+      </c>
+      <c r="U45" s="3">
+        <v>2.4885381870705521</v>
+      </c>
+      <c r="W45" s="3">
+        <f>M45-0.2</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="46" spans="11:25">
+      <c r="K46" s="6">
+        <v>14.703611457036114</v>
+      </c>
+      <c r="L46" s="6">
+        <v>73.597667638483955</v>
+      </c>
+      <c r="P46" s="16"/>
+      <c r="Q46" s="16"/>
+      <c r="R46" s="16"/>
+      <c r="S46" s="16"/>
+    </row>
+    <row r="47" spans="11:25">
+      <c r="K47" s="6">
+        <v>7.996124031007751</v>
+      </c>
+      <c r="L47" s="6">
+        <v>30.030456852791875</v>
+      </c>
+      <c r="M47" s="3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N47" s="3">
+        <f t="shared" si="2"/>
+        <v>3.7556266931751354</v>
+      </c>
+      <c r="P47" s="16">
+        <f>K47*$Y$28/(L47*$Y$27)</f>
+        <v>1.3248559147384777</v>
+      </c>
+      <c r="Q47" s="16">
+        <f>-$Y$30/LN((P47-1)/(P47*$Z$27-$Z$28))</f>
+        <v>3.7388090681306001</v>
+      </c>
+      <c r="R47" s="16">
+        <f>M47*$Y$28/(N47*$Y$27)</f>
+        <v>1.324855914738478</v>
+      </c>
+      <c r="S47" s="16">
+        <f>-$Y$30/LN((R47-1)/(R47*$Z$27-$Z$28))</f>
+        <v>3.7388090681306001</v>
+      </c>
+      <c r="U47" s="3">
+        <v>3.7388090681306001</v>
+      </c>
+      <c r="W47" s="3">
+        <f>M47-0.2</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="49" spans="13:19">
+      <c r="O49" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="50" spans="13:19">
+      <c r="M50" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="N50" s="3">
+        <f>STDEV(N27:N47)</f>
+        <v>0.5816202690505522</v>
+      </c>
+      <c r="O50" s="3">
+        <f>N51/N50</f>
+        <v>6.9020389730061744</v>
+      </c>
+      <c r="R50" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="S50" s="3">
+        <f>STDEV(S27:S47)</f>
+        <v>2.3828250851557571</v>
+      </c>
+    </row>
+    <row r="51" spans="13:19">
+      <c r="M51" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="N51" s="3">
+        <f>AVERAGE(N27:N47)</f>
+        <v>4.0143657644772484</v>
+      </c>
+      <c r="R51" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="S51" s="3">
+        <f>AVERAGE(S27:S47)</f>
+        <v>3.1044045457849361</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -4862,8 +7716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AI26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="AA13" sqref="AA13"/>
+    <sheetView topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AD23" sqref="AD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7873,67 +10727,67 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E23">
-    <cfRule type="cellIs" dxfId="106" priority="20" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="108" priority="20" operator="greaterThan">
       <formula>$D2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C23">
-    <cfRule type="cellIs" dxfId="105" priority="19" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="107" priority="19" operator="greaterThan">
       <formula>$B2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G23">
-    <cfRule type="cellIs" dxfId="104" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="106" priority="14" operator="greaterThan">
       <formula>$F2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I23">
-    <cfRule type="cellIs" dxfId="103" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="105" priority="13" operator="greaterThan">
       <formula>$H2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K23">
-    <cfRule type="cellIs" dxfId="102" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="104" priority="12" operator="greaterThan">
       <formula>$J2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M23 Z2:AA23">
-    <cfRule type="cellIs" dxfId="101" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="103" priority="11" operator="greaterThan">
       <formula>$L2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC2:AI23">
-    <cfRule type="cellIs" dxfId="100" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="102" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O23">
-    <cfRule type="cellIs" dxfId="99" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="101" priority="7" operator="greaterThan">
       <formula>$N2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q23">
-    <cfRule type="cellIs" dxfId="98" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="100" priority="6" operator="greaterThan">
       <formula>$P2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S23">
-    <cfRule type="cellIs" dxfId="97" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="99" priority="4" operator="greaterThan">
       <formula>$R2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2:U23">
-    <cfRule type="cellIs" dxfId="96" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="98" priority="3" operator="greaterThan">
       <formula>$T2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W2:W23">
-    <cfRule type="cellIs" dxfId="95" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="97" priority="2" operator="greaterThan">
       <formula>$V2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y2:Y23">
-    <cfRule type="cellIs" dxfId="94" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="96" priority="1" operator="greaterThan">
       <formula>$X2</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Worked on excel analysis of post contrast data
</commit_message>
<xml_diff>
--- a/Other files/Pacientes_sinais2e10.xlsx
+++ b/Other files/Pacientes_sinais2e10.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="106">
   <si>
     <t>Código</t>
   </si>
@@ -335,6 +335,12 @@
   <si>
     <t>SNR</t>
   </si>
+  <si>
+    <t>t = tan /2</t>
+  </si>
+  <si>
+    <t>Helms</t>
+  </si>
 </sst>
 </file>
 
@@ -342,7 +348,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="170" formatCode="0.00000"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -478,7 +484,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -488,31 +494,7 @@
     <cellStyle name="Input" xfId="3" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="143">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="141">
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
@@ -2344,23 +2326,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="77041024"/>
-        <c:axId val="77039488"/>
+        <c:axId val="97614848"/>
+        <c:axId val="97641216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="77041024"/>
+        <c:axId val="97614848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77039488"/>
+        <c:crossAx val="97641216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="77039488"/>
+        <c:axId val="97641216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2368,7 +2350,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77041024"/>
+        <c:crossAx val="97614848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2381,7 +2363,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2838,23 +2820,165 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="101579008"/>
-        <c:axId val="81543168"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>B*x</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Rescaled!$P$2:$P$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Rescaled!$R$2:$R$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25.200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>29.400000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>33.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>37.800000000000004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>46.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>50.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>58.800000000000004</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>67.2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>71.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>75.600000000000009</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>79.8</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>84</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="98379648"/>
+        <c:axId val="98381184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="101579008"/>
+        <c:axId val="98379648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81543168"/>
+        <c:crossAx val="98381184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="81543168"/>
+        <c:axId val="98381184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2862,7 +2986,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101579008"/>
+        <c:crossAx val="98379648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2875,7 +2999,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2892,6 +3016,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>S_10 valores</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575">
               <a:noFill/>
@@ -3162,23 +3289,161 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="82361344"/>
-        <c:axId val="82372096"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Helms</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Rescaled!$X$28:$X$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Rescaled!$Y$28:$Y$47</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1.9096253597885742</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.83623272263655513</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6600763646406491</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.59103041519718136</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.8993836552431977</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.5376036019516839</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.8665013658210712</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.3778865608202484</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.6276981722017112</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.2217351239820298</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.200565308077219</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.4702631825429489</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.198524609666793</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.9289860295100238</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.8987652257913643</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.6283127156830597</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.6307823880651098</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.8705886023000229</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="98416896"/>
+        <c:axId val="98422784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="82361344"/>
+        <c:axId val="98416896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82372096"/>
+        <c:crossAx val="98422784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="82372096"/>
+        <c:axId val="98422784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3186,7 +3451,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82361344"/>
+        <c:crossAx val="98416896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3199,7 +3464,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3306,48 +3571,48 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q23" totalsRowShown="0" headerRowDxfId="142" dataDxfId="141">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q23" totalsRowShown="0" headerRowDxfId="140" dataDxfId="139">
   <tableColumns count="17">
-    <tableColumn id="2" name="Código" dataDxfId="140"/>
-    <tableColumn id="16" name="Rescale A_2" dataDxfId="139"/>
-    <tableColumn id="17" name="Rescale B_2" dataDxfId="138"/>
-    <tableColumn id="18" name="Rescale A_10" dataDxfId="137"/>
-    <tableColumn id="19" name="Rescale B_10" dataDxfId="136"/>
-    <tableColumn id="1" name="2 - Fígado A" dataDxfId="135"/>
-    <tableColumn id="3" name="10 - Fígado A" dataDxfId="134"/>
-    <tableColumn id="4" name="2 - Fígado B" dataDxfId="133"/>
-    <tableColumn id="5" name="10 - Fígado B" dataDxfId="132"/>
-    <tableColumn id="6" name="2 - Fígado C" dataDxfId="131"/>
-    <tableColumn id="7" name="10 - Fígado C" dataDxfId="130"/>
-    <tableColumn id="8" name="2 - Rim " dataDxfId="129"/>
-    <tableColumn id="9" name="10 - Rim" dataDxfId="128"/>
-    <tableColumn id="10" name="2 - Gordura A" dataDxfId="127"/>
-    <tableColumn id="11" name="10 - Gordura A" dataDxfId="126"/>
-    <tableColumn id="12" name="2 - Gordura B" dataDxfId="125"/>
-    <tableColumn id="13" name="10 - Gordura B" dataDxfId="124"/>
+    <tableColumn id="2" name="Código" dataDxfId="138"/>
+    <tableColumn id="16" name="Rescale A_2" dataDxfId="137"/>
+    <tableColumn id="17" name="Rescale B_2" dataDxfId="136"/>
+    <tableColumn id="18" name="Rescale A_10" dataDxfId="135"/>
+    <tableColumn id="19" name="Rescale B_10" dataDxfId="134"/>
+    <tableColumn id="1" name="2 - Fígado A" dataDxfId="133"/>
+    <tableColumn id="3" name="10 - Fígado A" dataDxfId="132"/>
+    <tableColumn id="4" name="2 - Fígado B" dataDxfId="131"/>
+    <tableColumn id="5" name="10 - Fígado B" dataDxfId="130"/>
+    <tableColumn id="6" name="2 - Fígado C" dataDxfId="129"/>
+    <tableColumn id="7" name="10 - Fígado C" dataDxfId="128"/>
+    <tableColumn id="8" name="2 - Rim " dataDxfId="127"/>
+    <tableColumn id="9" name="10 - Rim" dataDxfId="126"/>
+    <tableColumn id="10" name="2 - Gordura A" dataDxfId="125"/>
+    <tableColumn id="11" name="10 - Gordura A" dataDxfId="124"/>
+    <tableColumn id="12" name="2 - Gordura B" dataDxfId="123"/>
+    <tableColumn id="13" name="10 - Gordura B" dataDxfId="122"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table511" displayName="Table511" ref="K2:Q20" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table511" displayName="Table511" ref="K2:Q20" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="K2:Q20"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Paciente" dataDxfId="8"/>
-    <tableColumn id="2" name="Fígado A" dataDxfId="7"/>
-    <tableColumn id="3" name="Fígado B" dataDxfId="6"/>
-    <tableColumn id="4" name="Fígado C" dataDxfId="5"/>
-    <tableColumn id="5" name="Rim" dataDxfId="4"/>
-    <tableColumn id="6" name="Gordura A" dataDxfId="3"/>
-    <tableColumn id="7" name="Gordura B" dataDxfId="2"/>
+    <tableColumn id="1" name="Paciente" dataDxfId="6"/>
+    <tableColumn id="2" name="Fígado A" dataDxfId="5"/>
+    <tableColumn id="3" name="Fígado B" dataDxfId="4"/>
+    <tableColumn id="4" name="Fígado C" dataDxfId="3"/>
+    <tableColumn id="5" name="Rim" dataDxfId="2"/>
+    <tableColumn id="6" name="Gordura A" dataDxfId="1"/>
+    <tableColumn id="7" name="Gordura B" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:M23" totalsRowShown="0" headerRowDxfId="123" dataDxfId="122">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:M23" totalsRowShown="0" headerRowDxfId="121" dataDxfId="120">
   <autoFilter ref="A1:M23">
     <filterColumn colId="1"/>
     <filterColumn colId="2"/>
@@ -3363,41 +3628,41 @@
     <filterColumn colId="12"/>
   </autoFilter>
   <tableColumns count="13">
-    <tableColumn id="1" name="Código" dataDxfId="121"/>
-    <tableColumn id="2" name="2 - Fígado A" dataDxfId="120">
+    <tableColumn id="1" name="Código" dataDxfId="119"/>
+    <tableColumn id="2" name="2 - Fígado A" dataDxfId="118">
       <calculatedColumnFormula>Table1[[#This Row],[2 - Fígado A]]/Table1[[#This Row],[Rescale A_2]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="10 - Fígado A" dataDxfId="119">
+    <tableColumn id="3" name="10 - Fígado A" dataDxfId="117">
       <calculatedColumnFormula>Table1[[#This Row],[10 - Fígado A]]/Table1[[#This Row],[Rescale A_10]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="2 - Fígado B" dataDxfId="118">
+    <tableColumn id="7" name="2 - Fígado B" dataDxfId="116">
       <calculatedColumnFormula>Table1[[#This Row],[2 - Fígado B]]/Table1[[#This Row],[Rescale A_2]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="10 - Fígado B" dataDxfId="117">
+    <tableColumn id="8" name="10 - Fígado B" dataDxfId="115">
       <calculatedColumnFormula>Table1[[#This Row],[10 - Fígado B]]/Table1[[#This Row],[Rescale A_10]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="2 - Fígado C" dataDxfId="116">
+    <tableColumn id="9" name="2 - Fígado C" dataDxfId="114">
       <calculatedColumnFormula>Table1[[#This Row],[2 - Fígado C]]/Table1[[#This Row],[Rescale A_2]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="10 - Fígado C" dataDxfId="115">
+    <tableColumn id="10" name="10 - Fígado C" dataDxfId="113">
       <calculatedColumnFormula>Table1[[#This Row],[10 - Fígado C]]/Table1[[#This Row],[Rescale A_10]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="2 - Rim " dataDxfId="114">
+    <tableColumn id="11" name="2 - Rim " dataDxfId="112">
       <calculatedColumnFormula>Table1[[#This Row],[2 - Rim ]]/Table1[[#This Row],[Rescale A_2]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="10 - Rim" dataDxfId="113">
+    <tableColumn id="12" name="10 - Rim" dataDxfId="111">
       <calculatedColumnFormula>Table1[[#This Row],[10 - Rim]]/Table1[[#This Row],[Rescale A_10]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="2 - Gordura A" dataDxfId="112">
+    <tableColumn id="13" name="2 - Gordura A" dataDxfId="110">
       <calculatedColumnFormula>Table1[[#This Row],[2 - Gordura A]]/Table1[[#This Row],[Rescale A_2]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="10 - Gordura A" dataDxfId="111">
+    <tableColumn id="14" name="10 - Gordura A" dataDxfId="109">
       <calculatedColumnFormula>Table1[[#This Row],[10 - Gordura A]]/Table1[[#This Row],[Rescale A_10]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="2 - Gordura B" dataDxfId="110">
+    <tableColumn id="15" name="2 - Gordura B" dataDxfId="108">
       <calculatedColumnFormula>Table1[[#This Row],[2 - Gordura B]]/Table1[[#This Row],[Rescale A_2]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="10 - Gordura B" dataDxfId="109">
+    <tableColumn id="16" name="10 - Gordura B" dataDxfId="107">
       <calculatedColumnFormula>Table1[[#This Row],[10 - Gordura B]]/Table1[[#This Row],[Rescale A_10]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3406,79 +3671,79 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table11" displayName="Table11" ref="A1:Y23" totalsRowShown="0" headerRowDxfId="95" dataDxfId="94">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table11" displayName="Table11" ref="A1:Y23" totalsRowShown="0" headerRowDxfId="93" dataDxfId="92">
   <tableColumns count="25">
-    <tableColumn id="1" name="Código" dataDxfId="93"/>
-    <tableColumn id="2" name="2 - Fíg A - S/sin" dataDxfId="92">
+    <tableColumn id="1" name="Código" dataDxfId="91"/>
+    <tableColumn id="2" name="2 - Fíg A - S/sin" dataDxfId="90">
       <calculatedColumnFormula>Table4[[#This Row],[2 - Fígado A]]/SIN(Original!$B$25*PI()/180)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="10 - Fíg A - S/sin" dataDxfId="91">
+    <tableColumn id="3" name="10 - Fíg A - S/sin" dataDxfId="89">
       <calculatedColumnFormula>Table4[[#This Row],[10 - Fígado A]]/SIN(Original!$B$26*PI()/180)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="2 - Fíg A - S/tan" dataDxfId="90">
+    <tableColumn id="14" name="2 - Fíg A - S/tan" dataDxfId="88">
       <calculatedColumnFormula>Table4[[#This Row],[2 - Fígado A]]/TAN(Original!$B$25*PI()/180)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="10 - Fíg A - S/tan" dataDxfId="89">
+    <tableColumn id="15" name="10 - Fíg A - S/tan" dataDxfId="87">
       <calculatedColumnFormula>Table4[[#This Row],[10 - Fígado A]]/TAN(Original!$B$26*PI()/180)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="2 - Fíg B - S/sin" dataDxfId="88">
+    <tableColumn id="4" name="2 - Fíg B - S/sin" dataDxfId="86">
       <calculatedColumnFormula>Table4[[#This Row],[2 - Fígado B]]/SIN(Original!$B$25*PI()/180)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="10 - Fíg B - S/sin" dataDxfId="87">
+    <tableColumn id="5" name="10 - Fíg B - S/sin" dataDxfId="85">
       <calculatedColumnFormula>Table4[[#This Row],[10 - Fígado B]]/SIN(Original!$B$26*PI()/180)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="2 - Fíg B - S/tan" dataDxfId="86">
+    <tableColumn id="6" name="2 - Fíg B - S/tan" dataDxfId="84">
       <calculatedColumnFormula>Table4[[#This Row],[2 - Fígado B]]/TAN(Original!$B$25*PI()/180)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="10 - Fíg B - S/tan" dataDxfId="85">
+    <tableColumn id="7" name="10 - Fíg B - S/tan" dataDxfId="83">
       <calculatedColumnFormula>Table4[[#This Row],[10 - Fígado B]]/TAN(Original!$B$26*PI()/180)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="2 - Fíg C - S/sin" dataDxfId="84">
+    <tableColumn id="8" name="2 - Fíg C - S/sin" dataDxfId="82">
       <calculatedColumnFormula>Table4[[#This Row],[2 - Fígado C]]/SIN(Original!$B$25*PI()/180)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="10 - Fíg C - S/sin" dataDxfId="83">
+    <tableColumn id="9" name="10 - Fíg C - S/sin" dataDxfId="81">
       <calculatedColumnFormula>Table4[[#This Row],[10 - Fígado C]]/SIN(Original!$B$26*PI()/180)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="2 - Fíg C - S/tan" dataDxfId="82">
+    <tableColumn id="10" name="2 - Fíg C - S/tan" dataDxfId="80">
       <calculatedColumnFormula>Table4[[#This Row],[2 - Fígado C]]/TAN(Original!$B$25*PI()/180)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="10 - Fíg C - S/tan" dataDxfId="81">
+    <tableColumn id="11" name="10 - Fíg C - S/tan" dataDxfId="79">
       <calculatedColumnFormula>Table4[[#This Row],[10 - Fígado C]]/TAN(Original!$B$26*PI()/180)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="2 - Rim - S/sin" dataDxfId="80">
+    <tableColumn id="16" name="2 - Rim - S/sin" dataDxfId="78">
       <calculatedColumnFormula>Table4[[#This Row],[2 - Rim ]]/SIN(Original!$B$25*PI()/180)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="10 - Rim - S/sin" dataDxfId="79">
+    <tableColumn id="17" name="10 - Rim - S/sin" dataDxfId="77">
       <calculatedColumnFormula>Table4[[#This Row],[10 - Rim]]/SIN(Original!$B$26*PI()/180)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" name="2 - Rim - S/tan" dataDxfId="78">
+    <tableColumn id="18" name="2 - Rim - S/tan" dataDxfId="76">
       <calculatedColumnFormula>Table4[[#This Row],[2 - Rim ]]/TAN(Original!$B$25*PI()/180)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" name="10 - Rim - S/tan" dataDxfId="77">
+    <tableColumn id="19" name="10 - Rim - S/tan" dataDxfId="75">
       <calculatedColumnFormula>Table4[[#This Row],[10 - Rim]]/TAN(Original!$B$26*PI()/180)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" name="2 - Gord A - S/sin" dataDxfId="76">
+    <tableColumn id="20" name="2 - Gord A - S/sin" dataDxfId="74">
       <calculatedColumnFormula>Table4[[#This Row],[2 - Gordura A]]/SIN(Original!$B$25*PI()/180)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" name="10 - Gord A - S/sin" dataDxfId="75">
+    <tableColumn id="21" name="10 - Gord A - S/sin" dataDxfId="73">
       <calculatedColumnFormula>Table4[[#This Row],[10 - Gordura A]]/SIN(Original!$B$26*PI()/180)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" name="2 - Gord A - S/tan" dataDxfId="74">
+    <tableColumn id="22" name="2 - Gord A - S/tan" dataDxfId="72">
       <calculatedColumnFormula>Table4[[#This Row],[2 - Gordura A]]/TAN(Original!$B$25*PI()/180)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" name="10 - Gord A - S/tan" dataDxfId="73">
+    <tableColumn id="23" name="10 - Gord A - S/tan" dataDxfId="71">
       <calculatedColumnFormula>Table4[[#This Row],[10 - Gordura A]]/TAN(Original!$B$26*PI()/180)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" name="2 - Gord B - S/sin" dataDxfId="72">
+    <tableColumn id="24" name="2 - Gord B - S/sin" dataDxfId="70">
       <calculatedColumnFormula>Table4[[#This Row],[2 - Gordura B]]/SIN(Original!$B$25*PI()/180)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" name="10 - Gord B - S/sin" dataDxfId="71">
+    <tableColumn id="25" name="10 - Gord B - S/sin" dataDxfId="69">
       <calculatedColumnFormula>Table4[[#This Row],[10 - Gordura B]]/SIN(Original!$B$26*PI()/180)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" name="2 - Gord B - S/tan" dataDxfId="70">
+    <tableColumn id="26" name="2 - Gord B - S/tan" dataDxfId="68">
       <calculatedColumnFormula>Table4[[#This Row],[2 - Gordura B]]/TAN(Original!$B$25*PI()/180)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" name="10 - Gord B - S/tan" dataDxfId="69">
+    <tableColumn id="27" name="10 - Gord B - S/tan" dataDxfId="67">
       <calculatedColumnFormula>Table4[[#This Row],[10 - Gordura B]]/TAN(Original!$B$26*PI()/180)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3487,26 +3752,26 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="AC1:AI23" totalsRowShown="0" headerRowDxfId="68" dataDxfId="67">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="AC1:AI23" totalsRowShown="0" headerRowDxfId="66" dataDxfId="65">
   <autoFilter ref="AC1:AI23"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Código" dataDxfId="66"/>
-    <tableColumn id="2" name="T1 Fig A" dataDxfId="65">
+    <tableColumn id="1" name="Código" dataDxfId="64"/>
+    <tableColumn id="2" name="T1 Fig A" dataDxfId="63">
       <calculatedColumnFormula>-$B$26/LN((Table11[[#This Row],[2 - Fíg A - S/sin]]-Table11[[#This Row],[10 - Fíg A - S/sin]])/(Table11[[#This Row],[2 - Fíg A - S/tan]]-Table11[[#This Row],[10 - Fíg A - S/tan]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="T1 Fig B" dataDxfId="64">
+    <tableColumn id="3" name="T1 Fig B" dataDxfId="62">
       <calculatedColumnFormula>-$B$26/LN((Table11[[#This Row],[2 - Fíg B - S/sin]]-Table11[[#This Row],[10 - Fíg B - S/sin]])/(Table11[[#This Row],[2 - Fíg B - S/tan]]-Table11[[#This Row],[10 - Fíg B - S/tan]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="T1 Fig C" dataDxfId="63">
+    <tableColumn id="4" name="T1 Fig C" dataDxfId="61">
       <calculatedColumnFormula>-$B$26/LN((Table11[[#This Row],[2 - Fíg C - S/sin]]-Table11[[#This Row],[10 - Fíg C - S/sin]])/(Table11[[#This Row],[2 - Fíg C - S/tan]]-Table11[[#This Row],[10 - Fíg C - S/tan]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="T1 Rim" dataDxfId="62">
+    <tableColumn id="5" name="T1 Rim" dataDxfId="60">
       <calculatedColumnFormula>-$B$26/LN((N2-O2)/(P2-Q2))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="T1 Gord. A" dataDxfId="61">
+    <tableColumn id="6" name="T1 Gord. A" dataDxfId="59">
       <calculatedColumnFormula>-$B$26/LN((Table11[[#This Row],[2 - Gord B - S/sin]]-Table11[[#This Row],[10 - Gord B - S/sin]])/(Table11[[#This Row],[2 - Gord B - S/tan]]-Table11[[#This Row],[10 - Gord B - S/tan]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="T1 Gord. B" dataDxfId="60">
+    <tableColumn id="7" name="T1 Gord. B" dataDxfId="58">
       <calculatedColumnFormula>-$B$26/LN((V2-W2)/(X2-Y2))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3515,25 +3780,25 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A2:G24" totalsRowShown="0" headerRowDxfId="59" dataDxfId="58">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A2:G24" totalsRowShown="0" headerRowDxfId="57" dataDxfId="56">
   <tableColumns count="7">
-    <tableColumn id="1" name="Paciente" dataDxfId="57"/>
-    <tableColumn id="2" name="Fígado A" dataDxfId="56">
+    <tableColumn id="1" name="Paciente" dataDxfId="55"/>
+    <tableColumn id="2" name="Fígado A" dataDxfId="54">
       <calculatedColumnFormula>(Rescaled!C2-Rescaled!B2)/(Original!$B$26-Original!$B$25)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Fígado B" dataDxfId="55">
+    <tableColumn id="3" name="Fígado B" dataDxfId="53">
       <calculatedColumnFormula>(Rescaled!E2-Rescaled!D2)/(Original!$B$26-Original!$B$25)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Fígado C" dataDxfId="54">
+    <tableColumn id="4" name="Fígado C" dataDxfId="52">
       <calculatedColumnFormula>(Rescaled!G2-Rescaled!F2)/(Original!$B$26-Original!$B$25)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Rim" dataDxfId="53">
+    <tableColumn id="5" name="Rim" dataDxfId="51">
       <calculatedColumnFormula>(Rescaled!I2-Rescaled!H2)/(Original!$B$26-Original!$B$25)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Gordura A" dataDxfId="52">
+    <tableColumn id="6" name="Gordura A" dataDxfId="50">
       <calculatedColumnFormula>(Rescaled!K2-Rescaled!J2)/(Original!$B$26-Original!$B$25)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Gordura B" dataDxfId="51">
+    <tableColumn id="7" name="Gordura B" dataDxfId="49">
       <calculatedColumnFormula>(Rescaled!M2-Rescaled!L2)/(Original!$B$26-Original!$B$25)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3542,59 +3807,59 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="K2:Q22" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="K2:Q22" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
   <autoFilter ref="K2:Q22"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Paciente" dataDxfId="48"/>
-    <tableColumn id="2" name="Fígado A" dataDxfId="47"/>
-    <tableColumn id="3" name="Fígado B" dataDxfId="46"/>
-    <tableColumn id="4" name="Fígado C" dataDxfId="45"/>
-    <tableColumn id="5" name="Rim" dataDxfId="44"/>
-    <tableColumn id="6" name="Gordura A" dataDxfId="43"/>
-    <tableColumn id="7" name="Gordura B" dataDxfId="42"/>
+    <tableColumn id="1" name="Paciente" dataDxfId="46"/>
+    <tableColumn id="2" name="Fígado A" dataDxfId="45"/>
+    <tableColumn id="3" name="Fígado B" dataDxfId="44"/>
+    <tableColumn id="4" name="Fígado C" dataDxfId="43"/>
+    <tableColumn id="5" name="Rim" dataDxfId="42"/>
+    <tableColumn id="6" name="Gordura A" dataDxfId="41"/>
+    <tableColumn id="7" name="Gordura B" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table43" displayName="Table43" ref="A1:M23" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table43" displayName="Table43" ref="A1:M23" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
   <tableColumns count="13">
-    <tableColumn id="1" name="Código" dataDxfId="39"/>
-    <tableColumn id="2" name="2 - Fígado A" dataDxfId="38">
+    <tableColumn id="1" name="Código" dataDxfId="37"/>
+    <tableColumn id="2" name="2 - Fígado A" dataDxfId="36">
       <calculatedColumnFormula>Table1[[#This Row],[2 - Fígado A]]/Table1[[#This Row],[Rescale A_2]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="10 - Fígado A" dataDxfId="37">
+    <tableColumn id="3" name="10 - Fígado A" dataDxfId="35">
       <calculatedColumnFormula>Table1[[#This Row],[10 - Fígado A]]/Table1[[#This Row],[Rescale A_10]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="2 - Fígado B" dataDxfId="36">
+    <tableColumn id="7" name="2 - Fígado B" dataDxfId="34">
       <calculatedColumnFormula>Table1[[#This Row],[2 - Fígado B]]/Table1[[#This Row],[Rescale A_2]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="10 - Fígado B" dataDxfId="35">
+    <tableColumn id="8" name="10 - Fígado B" dataDxfId="33">
       <calculatedColumnFormula>Table1[[#This Row],[10 - Fígado B]]/Table1[[#This Row],[Rescale A_10]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="2 - Fígado C" dataDxfId="34">
+    <tableColumn id="9" name="2 - Fígado C" dataDxfId="32">
       <calculatedColumnFormula>Table1[[#This Row],[2 - Fígado C]]/Table1[[#This Row],[Rescale A_2]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="10 - Fígado C" dataDxfId="33">
+    <tableColumn id="10" name="10 - Fígado C" dataDxfId="31">
       <calculatedColumnFormula>Table1[[#This Row],[10 - Fígado C]]/Table1[[#This Row],[Rescale A_10]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="2 - Rim " dataDxfId="32">
+    <tableColumn id="11" name="2 - Rim " dataDxfId="30">
       <calculatedColumnFormula>Table1[[#This Row],[2 - Rim ]]/Table1[[#This Row],[Rescale A_2]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="10 - Rim" dataDxfId="31">
+    <tableColumn id="12" name="10 - Rim" dataDxfId="29">
       <calculatedColumnFormula>Table1[[#This Row],[10 - Rim]]/Table1[[#This Row],[Rescale A_10]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="2 - Gordura A" dataDxfId="30">
+    <tableColumn id="13" name="2 - Gordura A" dataDxfId="28">
       <calculatedColumnFormula>Table1[[#This Row],[2 - Gordura A]]/Table1[[#This Row],[Rescale A_2]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="10 - Gordura A" dataDxfId="29">
+    <tableColumn id="14" name="10 - Gordura A" dataDxfId="27">
       <calculatedColumnFormula>Table1[[#This Row],[10 - Gordura A]]/Table1[[#This Row],[Rescale A_10]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="2 - Gordura B" dataDxfId="28">
+    <tableColumn id="15" name="2 - Gordura B" dataDxfId="26">
       <calculatedColumnFormula>Table1[[#This Row],[2 - Gordura B]]/Table1[[#This Row],[Rescale A_2]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="10 - Gordura B" dataDxfId="27">
+    <tableColumn id="16" name="10 - Gordura B" dataDxfId="25">
       <calculatedColumnFormula>Table1[[#This Row],[10 - Gordura B]]/Table1[[#This Row],[Rescale A_10]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3603,21 +3868,21 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="P1:T23" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="P1:T23" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
   <tableColumns count="5">
-    <tableColumn id="1" name="A10 - Ideal (alpha)" dataDxfId="24">
+    <tableColumn id="1" name="A10 - Ideal (alpha)" dataDxfId="22">
       <calculatedColumnFormula>$B$25*Table43[[#This Row],[2 - Gordura A]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="A10 - 10ideal/10real (beta)" dataDxfId="23">
+    <tableColumn id="2" name="A10 - 10ideal/10real (beta)" dataDxfId="21">
       <calculatedColumnFormula>P2/Table43[[#This Row],[10 - Gordura A]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="B10 - Ideal (alpha)" dataDxfId="22">
+    <tableColumn id="3" name="B10 - Ideal (alpha)" dataDxfId="20">
       <calculatedColumnFormula>$B$25*Table43[[#This Row],[2 - Gordura B]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="B10 - 10ideal/10real (beta)" dataDxfId="21">
+    <tableColumn id="4" name="B10 - 10ideal/10real (beta)" dataDxfId="19">
       <calculatedColumnFormula>Table3[[#This Row],[B10 - Ideal (alpha)]]/Table43[[#This Row],[10 - Gordura B]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Avg Beta" dataDxfId="20">
+    <tableColumn id="5" name="Avg Beta" dataDxfId="18">
       <calculatedColumnFormula>AVERAGE(Table3[[#This Row],[B10 - 10ideal/10real (beta)]],Table3[[#This Row],[A10 - 10ideal/10real (beta)]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3626,25 +3891,25 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table610" displayName="Table610" ref="A2:G24" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table610" displayName="Table610" ref="A2:G24" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <tableColumns count="7">
-    <tableColumn id="1" name="Paciente" dataDxfId="17"/>
-    <tableColumn id="2" name="Fígado A" dataDxfId="16">
+    <tableColumn id="1" name="Paciente" dataDxfId="15"/>
+    <tableColumn id="2" name="Fígado A" dataDxfId="14">
       <calculatedColumnFormula>(Rescaled!C2-Rescaled!B2)/(Original!$B$26-Original!$B$25)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Fígado B" dataDxfId="15">
+    <tableColumn id="3" name="Fígado B" dataDxfId="13">
       <calculatedColumnFormula>(Rescaled!E2-Rescaled!D2)/(Original!$B$26-Original!$B$25)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Fígado C" dataDxfId="14">
+    <tableColumn id="4" name="Fígado C" dataDxfId="12">
       <calculatedColumnFormula>(Rescaled!G2-Rescaled!F2)/(Original!$B$26-Original!$B$25)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Rim" dataDxfId="13">
+    <tableColumn id="5" name="Rim" dataDxfId="11">
       <calculatedColumnFormula>(Rescaled!I2-Rescaled!H2)/(Original!$B$26-Original!$B$25)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" name="Gordura A" dataDxfId="12">
+    <tableColumn id="6" name="Gordura A" dataDxfId="10">
       <calculatedColumnFormula>(Rescaled!K2-Rescaled!J2)/(Original!$B$26-Original!$B$25)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" name="Gordura B" dataDxfId="11">
+    <tableColumn id="7" name="Gordura B" dataDxfId="9">
       <calculatedColumnFormula>(Rescaled!M2-Rescaled!L2)/(Original!$B$26-Original!$B$25)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4144,7 +4409,7 @@
         <v>10</v>
       </c>
       <c r="U3" s="4">
-        <f t="shared" ref="U3:U23" si="0">$X$2*T3</f>
+        <f t="shared" ref="U3:U18" si="0">$X$2*T3</f>
         <v>20</v>
       </c>
       <c r="V3" s="4">
@@ -5411,10 +5676,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Z51"/>
+  <dimension ref="A1:Y51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E19" workbookViewId="0">
-      <selection activeCell="P28" sqref="P28:S47"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J45" sqref="J45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5440,7 +5705,7 @@
     <col min="20" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:23">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -5481,7 +5746,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:23">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -5540,7 +5805,10 @@
         <f>$T$2*P2</f>
         <v>4.74</v>
       </c>
-      <c r="R2" s="4"/>
+      <c r="R2" s="4">
+        <f>P2*$T$3</f>
+        <v>4.2</v>
+      </c>
       <c r="S2" s="14" t="s">
         <v>90</v>
       </c>
@@ -5548,7 +5816,7 @@
         <v>4.74</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:23">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -5604,14 +5872,21 @@
         <v>2</v>
       </c>
       <c r="Q3" s="4">
-        <f t="shared" ref="Q3:Q23" si="0">$T$2*P3</f>
+        <f t="shared" ref="Q3:R20" si="0">$T$2*P3</f>
         <v>9.48</v>
       </c>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-      <c r="T3" s="4"/>
-    </row>
-    <row r="4" spans="1:20">
+      <c r="R3" s="4">
+        <f t="shared" ref="R3:R20" si="1">P3*$T$3</f>
+        <v>8.4</v>
+      </c>
+      <c r="S3" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="T3" s="15">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -5670,11 +5945,14 @@
         <f t="shared" si="0"/>
         <v>14.22</v>
       </c>
-      <c r="R4" s="4"/>
+      <c r="R4" s="4">
+        <f t="shared" si="1"/>
+        <v>12.600000000000001</v>
+      </c>
       <c r="S4" s="4"/>
       <c r="T4" s="4"/>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:23">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -5733,11 +6011,14 @@
         <f t="shared" si="0"/>
         <v>18.96</v>
       </c>
-      <c r="R5" s="4"/>
+      <c r="R5" s="4">
+        <f t="shared" si="1"/>
+        <v>16.8</v>
+      </c>
       <c r="S5" s="4"/>
       <c r="T5" s="4"/>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:23">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -5796,11 +6077,14 @@
         <f t="shared" si="0"/>
         <v>23.700000000000003</v>
       </c>
-      <c r="R6" s="4"/>
+      <c r="R6" s="4">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
       <c r="S6" s="4"/>
       <c r="T6" s="4"/>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:23">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -5859,11 +6143,14 @@
         <f t="shared" si="0"/>
         <v>28.44</v>
       </c>
-      <c r="R7" s="4"/>
+      <c r="R7" s="4">
+        <f t="shared" si="1"/>
+        <v>25.200000000000003</v>
+      </c>
       <c r="S7" s="4"/>
       <c r="T7" s="4"/>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:23">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -5922,11 +6209,14 @@
         <f t="shared" si="0"/>
         <v>33.18</v>
       </c>
-      <c r="R8" s="4"/>
+      <c r="R8" s="4">
+        <f t="shared" si="1"/>
+        <v>29.400000000000002</v>
+      </c>
       <c r="S8" s="4"/>
       <c r="T8" s="4"/>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:23">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -5985,11 +6275,14 @@
         <f t="shared" si="0"/>
         <v>37.92</v>
       </c>
-      <c r="R9" s="4"/>
+      <c r="R9" s="4">
+        <f t="shared" si="1"/>
+        <v>33.6</v>
+      </c>
       <c r="S9" s="4"/>
       <c r="T9" s="4"/>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:23">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -6048,11 +6341,14 @@
         <f t="shared" si="0"/>
         <v>42.660000000000004</v>
       </c>
-      <c r="R10" s="4"/>
+      <c r="R10" s="4">
+        <f t="shared" si="1"/>
+        <v>37.800000000000004</v>
+      </c>
       <c r="S10" s="4"/>
       <c r="T10" s="4"/>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:23">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -6111,11 +6407,14 @@
         <f t="shared" si="0"/>
         <v>47.400000000000006</v>
       </c>
-      <c r="R11" s="4"/>
+      <c r="R11" s="4">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
       <c r="S11" s="4"/>
       <c r="T11" s="4"/>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:23">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -6174,11 +6473,14 @@
         <f t="shared" si="0"/>
         <v>52.14</v>
       </c>
-      <c r="R12" s="4"/>
+      <c r="R12" s="4">
+        <f t="shared" si="1"/>
+        <v>46.2</v>
+      </c>
       <c r="S12" s="4"/>
       <c r="T12" s="4"/>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:23">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
@@ -6237,11 +6539,25 @@
         <f t="shared" si="0"/>
         <v>56.88</v>
       </c>
-      <c r="R13" s="4"/>
+      <c r="R13" s="4">
+        <f t="shared" si="1"/>
+        <v>50.400000000000006</v>
+      </c>
       <c r="S13" s="4"/>
-      <c r="T13" s="4"/>
-    </row>
-    <row r="14" spans="1:20">
+      <c r="T13" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="U13" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="V13" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="W13" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -6300,11 +6616,28 @@
         <f t="shared" si="0"/>
         <v>66.36</v>
       </c>
-      <c r="R14" s="4"/>
+      <c r="R14" s="4">
+        <f t="shared" si="1"/>
+        <v>58.800000000000004</v>
+      </c>
       <c r="S14" s="4"/>
-      <c r="T14" s="4"/>
-    </row>
-    <row r="15" spans="1:20">
+      <c r="T14" s="3">
+        <v>2</v>
+      </c>
+      <c r="U14" s="3">
+        <f>SIN(T14*PI()/180)</f>
+        <v>3.4899496702500969E-2</v>
+      </c>
+      <c r="V14" s="3">
+        <f>COS(T14*PI()/180)</f>
+        <v>0.99939082701909576</v>
+      </c>
+      <c r="W14" s="3">
+        <f>TAN(T14*PI()/180)/2</f>
+        <v>1.7460384745873865E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
@@ -6363,11 +6696,28 @@
         <f t="shared" si="0"/>
         <v>71.100000000000009</v>
       </c>
-      <c r="R15" s="4"/>
+      <c r="R15" s="4">
+        <f t="shared" si="1"/>
+        <v>63</v>
+      </c>
       <c r="S15" s="4"/>
-      <c r="T15" s="4"/>
-    </row>
-    <row r="16" spans="1:20">
+      <c r="T15" s="3">
+        <v>10</v>
+      </c>
+      <c r="U15" s="3">
+        <f>SIN(T15*PI()/180)</f>
+        <v>0.17364817766693033</v>
+      </c>
+      <c r="V15" s="3">
+        <f>COS(T15*PI()/180)</f>
+        <v>0.98480775301220802</v>
+      </c>
+      <c r="W15" s="3">
+        <f>TAN(T15*PI()/180)/2</f>
+        <v>8.8163490354232488E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
@@ -6426,11 +6776,13 @@
         <f t="shared" si="0"/>
         <v>75.84</v>
       </c>
-      <c r="R16" s="4"/>
+      <c r="R16" s="4">
+        <f t="shared" si="1"/>
+        <v>67.2</v>
+      </c>
       <c r="S16" s="4"/>
-      <c r="T16" s="4"/>
-    </row>
-    <row r="17" spans="1:26">
+    </row>
+    <row r="17" spans="1:25">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
@@ -6489,11 +6841,19 @@
         <f t="shared" si="0"/>
         <v>80.58</v>
       </c>
-      <c r="R17" s="4"/>
+      <c r="R17" s="4">
+        <f t="shared" si="1"/>
+        <v>71.400000000000006</v>
+      </c>
       <c r="S17" s="4"/>
-      <c r="T17" s="4"/>
-    </row>
-    <row r="18" spans="1:26">
+      <c r="T17" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="U17" s="3">
+        <v>0.16200000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
@@ -6552,11 +6912,13 @@
         <f t="shared" si="0"/>
         <v>85.320000000000007</v>
       </c>
-      <c r="R18" s="4"/>
+      <c r="R18" s="4">
+        <f t="shared" si="1"/>
+        <v>75.600000000000009</v>
+      </c>
       <c r="S18" s="4"/>
-      <c r="T18" s="4"/>
-    </row>
-    <row r="19" spans="1:26">
+    </row>
+    <row r="19" spans="1:25">
       <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
@@ -6615,11 +6977,13 @@
         <f t="shared" si="0"/>
         <v>90.06</v>
       </c>
-      <c r="R19" s="4"/>
+      <c r="R19" s="4">
+        <f t="shared" si="1"/>
+        <v>79.8</v>
+      </c>
       <c r="S19" s="4"/>
-      <c r="T19" s="4"/>
-    </row>
-    <row r="20" spans="1:26">
+    </row>
+    <row r="20" spans="1:25">
       <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
@@ -6678,11 +7042,13 @@
         <f t="shared" si="0"/>
         <v>94.800000000000011</v>
       </c>
-      <c r="R20" s="4"/>
+      <c r="R20" s="4">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
       <c r="S20" s="4"/>
-      <c r="T20" s="4"/>
-    </row>
-    <row r="21" spans="1:26">
+    </row>
+    <row r="21" spans="1:25">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
@@ -6738,9 +7104,8 @@
       <c r="Q21" s="4"/>
       <c r="R21" s="4"/>
       <c r="S21" s="4"/>
-      <c r="T21" s="4"/>
-    </row>
-    <row r="22" spans="1:26">
+    </row>
+    <row r="22" spans="1:25">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
@@ -6796,9 +7161,16 @@
       <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
       <c r="S22" s="4"/>
-      <c r="T22" s="4"/>
-    </row>
-    <row r="23" spans="1:26">
+      <c r="T22" s="3">
+        <f>U15/U14</f>
+        <v>4.9756642380027891</v>
+      </c>
+      <c r="U22" s="3">
+        <f>T22/T2</f>
+        <v>1.0497181936714743</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25">
       <c r="A23" s="3" t="s">
         <v>22</v>
       </c>
@@ -6854,9 +7226,13 @@
       <c r="Q23" s="4"/>
       <c r="R23" s="4"/>
       <c r="S23" s="4"/>
-      <c r="T23" s="4"/>
-    </row>
-    <row r="26" spans="1:26">
+    </row>
+    <row r="25" spans="1:25">
+      <c r="Y25" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25">
       <c r="K26" s="3">
         <v>2</v>
       </c>
@@ -6881,36 +7257,16 @@
       <c r="S26" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="X26" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="Y26" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="Z26" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="27" spans="1:26">
+    </row>
+    <row r="27" spans="1:25">
       <c r="K27" s="6">
         <v>3.275167785234899</v>
       </c>
       <c r="L27" s="6">
         <v>37.717647058823538</v>
       </c>
-      <c r="X27" s="3">
-        <v>2</v>
-      </c>
-      <c r="Y27" s="3">
-        <f>SIN(X27*PI()/180)</f>
-        <v>3.4899496702500969E-2</v>
-      </c>
-      <c r="Z27" s="3">
-        <f>COS(X27*PI()/180)</f>
-        <v>0.99939082701909576</v>
-      </c>
-    </row>
-    <row r="28" spans="1:26">
+    </row>
+    <row r="28" spans="1:25">
       <c r="K28" s="6">
         <v>11.490523968784837</v>
       </c>
@@ -6918,49 +7274,46 @@
         <v>49.698113207547166</v>
       </c>
       <c r="M28" s="3">
-        <f t="shared" ref="M28:M47" si="1">K28/K28</f>
+        <f t="shared" ref="M28:M47" si="2">K28/K28</f>
         <v>1</v>
       </c>
       <c r="N28" s="3">
-        <f t="shared" ref="N28:N47" si="2">L28/K28</f>
+        <f t="shared" ref="N28:N47" si="3">L28/K28</f>
         <v>4.3251389877917736</v>
       </c>
       <c r="P28" s="16">
-        <f>K28*$Y$28/(L28*$Y$27)</f>
+        <f>K28*$U$15/(L28*$U$14)</f>
         <v>1.1504056290554365</v>
       </c>
       <c r="Q28" s="16">
-        <f>-$Y$30/LN((P28-1)/(P28*$Z$27-$Z$28))</f>
+        <f>-$U$17/LN((P28-1)/(P28*$V$14-$V$15))</f>
         <v>1.7611436189939376</v>
       </c>
       <c r="R28" s="16">
-        <f>M28*$Y$28/(N28*$Y$27)</f>
+        <f>M28*$U$15/(N28*$U$14)</f>
         <v>1.1504056290554363</v>
       </c>
       <c r="S28" s="16">
-        <f>-$Y$30/LN((R28-1)/(R28*$Z$27-$Z$28))</f>
+        <f>-$U$17/LN((R28-1)/(R28*$V$14-$V$15))</f>
         <v>1.7611436189939353</v>
       </c>
-      <c r="U28" s="3">
+      <c r="U28" s="16">
         <v>1.7611436189939329</v>
       </c>
       <c r="W28" s="3">
-        <f>M28-0.2</f>
+        <f t="shared" ref="W28:X36" si="4">M28-0.2</f>
         <v>0.8</v>
       </c>
       <c r="X28" s="3">
-        <v>10</v>
+        <f>W28-0.3</f>
+        <v>0.5</v>
       </c>
       <c r="Y28" s="3">
-        <f>SIN(X28*PI()/180)</f>
-        <v>0.17364817766693033</v>
-      </c>
-      <c r="Z28" s="3">
-        <f>COS(X28*PI()/180)</f>
-        <v>0.98480775301220802</v>
-      </c>
-    </row>
-    <row r="29" spans="1:26">
+        <f>$U$17*(((M28/$W$14-N28/$W$15)+(N28*$W$15-M28*$W$14))/(2*(N28*$W$15-M28*$W$14)))</f>
+        <v>1.9096253597885742</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25">
       <c r="K29" s="6">
         <v>8.8557347670250888</v>
       </c>
@@ -6968,38 +7321,46 @@
         <v>41.8125</v>
       </c>
       <c r="M29" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N29" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.7215167459273504</v>
       </c>
       <c r="P29" s="16">
-        <f>K29*$Y$28/(L29*$Y$27)</f>
+        <f>K29*$U$15/(L29*$U$14)</f>
         <v>1.0538275104699477</v>
       </c>
       <c r="Q29" s="16">
-        <f>-$Y$30/LN((P29-1)/(P29*$Z$27-$Z$28))</f>
+        <f>-$U$17/LN((P29-1)/(P29*$V$14-$V$15))</f>
         <v>0.67707794546015254</v>
       </c>
       <c r="R29" s="16">
-        <f>M29*$Y$28/(N29*$Y$27)</f>
+        <f>M29*$U$15/(N29*$U$14)</f>
         <v>1.0538275104699477</v>
       </c>
       <c r="S29" s="16">
-        <f>-$Y$30/LN((R29-1)/(R29*$Z$27-$Z$28))</f>
+        <f>-$U$17/LN((R29-1)/(R29*$V$14-$V$15))</f>
         <v>0.67707794546015254</v>
       </c>
-      <c r="U29" s="3">
+      <c r="U29" s="16">
         <v>0.67707794546015576</v>
       </c>
       <c r="W29" s="3">
-        <f>M29-0.2</f>
+        <f t="shared" si="4"/>
         <v>0.8</v>
       </c>
-    </row>
-    <row r="30" spans="1:26">
+      <c r="X29" s="3">
+        <f t="shared" ref="X29:X47" si="5">W29-0.3</f>
+        <v>0.5</v>
+      </c>
+      <c r="Y29" s="3">
+        <f t="shared" ref="Y29:Y47" si="6">$U$17*(((M29/$W$14-N29/$W$15)+(N29*$W$15-M29*$W$14))/(2*(N29*$W$15-M29*$W$14)))</f>
+        <v>0.83623272263655513</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25">
       <c r="K30" s="6">
         <v>9.6373626373626369</v>
       </c>
@@ -7007,44 +7368,46 @@
         <v>42.510067114093964</v>
       </c>
       <c r="M30" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N30" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.4109647746665344</v>
       </c>
       <c r="P30" s="16">
-        <f>K30*$Y$28/(L30*$Y$27)</f>
+        <f>K30*$U$15/(L30*$U$14)</f>
         <v>1.1280217576389384</v>
       </c>
       <c r="Q30" s="16">
-        <f>-$Y$30/LN((P30-1)/(P30*$Z$27-$Z$28))</f>
+        <f>-$U$17/LN((P30-1)/(P30*$V$14-$V$15))</f>
         <v>1.5093617935882717</v>
       </c>
       <c r="R30" s="16">
-        <f>M30*$Y$28/(N30*$Y$27)</f>
+        <f>M30*$U$15/(N30*$U$14)</f>
         <v>1.1280217576389386</v>
       </c>
       <c r="S30" s="16">
-        <f>-$Y$30/LN((R30-1)/(R30*$Z$27-$Z$28))</f>
+        <f>-$U$17/LN((R30-1)/(R30*$V$14-$V$15))</f>
         <v>1.5093617935882735</v>
       </c>
-      <c r="U30" s="3">
+      <c r="U30" s="16">
         <v>1.5093617935882702</v>
       </c>
       <c r="W30" s="3">
-        <f>M30-0.2</f>
+        <f t="shared" si="4"/>
         <v>0.8</v>
       </c>
-      <c r="X30" s="3" t="s">
-        <v>71</v>
+      <c r="X30" s="3">
+        <f t="shared" si="5"/>
+        <v>0.5</v>
       </c>
       <c r="Y30" s="3">
-        <v>0.16200000000000001</v>
-      </c>
-    </row>
-    <row r="31" spans="1:26">
+        <f t="shared" si="6"/>
+        <v>1.6600763646406491</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25">
       <c r="K31" s="6">
         <v>7.3270440251572317</v>
       </c>
@@ -7052,38 +7415,46 @@
         <v>35.338235294117652</v>
       </c>
       <c r="M31" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N31" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.8229866195405213</v>
       </c>
       <c r="P31" s="16">
-        <f>K31*$Y$28/(L31*$Y$27)</f>
+        <f>K31*$U$15/(L31*$U$14)</f>
         <v>1.0316562392778965</v>
       </c>
       <c r="Q31" s="16">
-        <f>-$Y$30/LN((P31-1)/(P31*$Z$27-$Z$28))</f>
+        <f>-$U$17/LN((P31-1)/(P31*$V$14-$V$15))</f>
         <v>0.4280301934750958</v>
       </c>
       <c r="R31" s="16">
-        <f>M31*$Y$28/(N31*$Y$27)</f>
+        <f>M31*$U$15/(N31*$U$14)</f>
         <v>1.0316562392778965</v>
       </c>
       <c r="S31" s="16">
-        <f>-$Y$30/LN((R31-1)/(R31*$Z$27-$Z$28))</f>
+        <f>-$U$17/LN((R31-1)/(R31*$V$14-$V$15))</f>
         <v>0.4280301934750958</v>
       </c>
-      <c r="U31" s="3">
+      <c r="U31" s="16">
         <v>0.42803019347509341</v>
       </c>
       <c r="W31" s="3">
-        <f>M31-0.2</f>
+        <f t="shared" si="4"/>
         <v>0.8</v>
       </c>
-    </row>
-    <row r="32" spans="1:26">
+      <c r="X31" s="3">
+        <f t="shared" si="5"/>
+        <v>0.5</v>
+      </c>
+      <c r="Y31" s="3">
+        <f t="shared" si="6"/>
+        <v>0.59103041519718136</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25">
       <c r="K32" s="6">
         <v>20.40360610263523</v>
       </c>
@@ -7091,35 +7462,43 @@
         <v>67.559907834101381</v>
       </c>
       <c r="M32" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N32" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.311174872434715</v>
       </c>
       <c r="P32" s="16">
-        <f>K32*$Y$28/(L32*$Y$27)</f>
+        <f>K32*$U$15/(L32*$U$14)</f>
         <v>1.5026884503820153</v>
       </c>
       <c r="Q32" s="16">
-        <f>-$Y$30/LN((P32-1)/(P32*$Z$27-$Z$28))</f>
+        <f>-$U$17/LN((P32-1)/(P32*$V$14-$V$15))</f>
         <v>5.7846483968471025</v>
       </c>
       <c r="R32" s="16">
-        <f>M32*$Y$28/(N32*$Y$27)</f>
+        <f>M32*$U$15/(N32*$U$14)</f>
         <v>1.5026884503820153</v>
       </c>
       <c r="S32" s="16">
-        <f>-$Y$30/LN((R32-1)/(R32*$Z$27-$Z$28))</f>
+        <f>-$U$17/LN((R32-1)/(R32*$V$14-$V$15))</f>
         <v>5.7846483968471025</v>
       </c>
-      <c r="U32" s="3">
+      <c r="U32" s="16">
         <v>5.7846483968471736</v>
       </c>
       <c r="W32" s="3">
-        <f>M32-0.2</f>
+        <f t="shared" si="4"/>
         <v>0.8</v>
+      </c>
+      <c r="X32" s="3">
+        <f t="shared" si="5"/>
+        <v>0.5</v>
+      </c>
+      <c r="Y32" s="3">
+        <f t="shared" si="6"/>
+        <v>5.8993836552431977</v>
       </c>
     </row>
     <row r="33" spans="11:25">
@@ -7130,35 +7509,43 @@
         <v>34.845217391304352</v>
       </c>
       <c r="M33" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N33" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.7413740115141598</v>
       </c>
       <c r="P33" s="16">
-        <f>K33*$Y$28/(L33*$Y$27)</f>
+        <f>K33*$U$15/(L33*$U$14)</f>
         <v>1.8150256831443989</v>
       </c>
       <c r="Q33" s="16">
-        <f>-$Y$30/LN((P33-1)/(P33*$Z$27-$Z$28))</f>
+        <f>-$U$17/LN((P33-1)/(P33*$V$14-$V$15))</f>
         <v>9.4538129635987005</v>
       </c>
       <c r="R33" s="16">
-        <f>M33*$Y$28/(N33*$Y$27)</f>
+        <f>M33*$U$15/(N33*$U$14)</f>
         <v>1.8150256831443987</v>
       </c>
       <c r="S33" s="16">
-        <f>-$Y$30/LN((R33-1)/(R33*$Z$27-$Z$28))</f>
+        <f>-$U$17/LN((R33-1)/(R33*$V$14-$V$15))</f>
         <v>9.4538129635987005</v>
       </c>
-      <c r="U33" s="3">
+      <c r="U33" s="16">
         <v>9.4538129635988248</v>
       </c>
       <c r="W33" s="3">
-        <f>M33-0.2</f>
+        <f t="shared" si="4"/>
         <v>0.8</v>
+      </c>
+      <c r="X33" s="3">
+        <f t="shared" si="5"/>
+        <v>0.5</v>
+      </c>
+      <c r="Y33" s="3">
+        <f t="shared" si="6"/>
+        <v>9.5376036019516839</v>
       </c>
     </row>
     <row r="34" spans="11:25">
@@ -7169,35 +7556,43 @@
         <v>46.91348088531187</v>
       </c>
       <c r="M34" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N34" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.3397195316109176</v>
       </c>
       <c r="P34" s="16">
-        <f>K34*$Y$28/(L34*$Y$27)</f>
+        <f>K34*$U$15/(L34*$U$14)</f>
         <v>1.1465405083806894</v>
       </c>
       <c r="Q34" s="16">
-        <f>-$Y$30/LN((P34-1)/(P34*$Z$27-$Z$28))</f>
+        <f>-$U$17/LN((P34-1)/(P34*$V$14-$V$15))</f>
         <v>1.7176378536963226</v>
       </c>
       <c r="R34" s="16">
-        <f>M34*$Y$28/(N34*$Y$27)</f>
+        <f>M34*$U$15/(N34*$U$14)</f>
         <v>1.1465405083806894</v>
       </c>
       <c r="S34" s="16">
-        <f>-$Y$30/LN((R34-1)/(R34*$Z$27-$Z$28))</f>
+        <f>-$U$17/LN((R34-1)/(R34*$V$14-$V$15))</f>
         <v>1.7176378536963226</v>
       </c>
-      <c r="U34" s="3">
+      <c r="U34" s="16">
         <v>1.7176378536963004</v>
       </c>
       <c r="W34" s="3">
-        <f>M34-0.2</f>
+        <f t="shared" si="4"/>
         <v>0.8</v>
+      </c>
+      <c r="X34" s="3">
+        <f t="shared" si="5"/>
+        <v>0.5</v>
+      </c>
+      <c r="Y34" s="3">
+        <f t="shared" si="6"/>
+        <v>1.8665013658210712</v>
       </c>
     </row>
     <row r="35" spans="11:25">
@@ -7208,43 +7603,43 @@
         <v>79.766756032171571</v>
       </c>
       <c r="M35" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N35" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.5124205741771721</v>
       </c>
       <c r="P35" s="16">
-        <f>K35*$Y$28/(L35*$Y$27)</f>
+        <f>K35*$U$15/(L35*$U$14)</f>
         <v>1.1026596825829094</v>
       </c>
       <c r="Q35" s="16">
-        <f>-$Y$30/LN((P35-1)/(P35*$Z$27-$Z$28))</f>
+        <f>-$U$17/LN((P35-1)/(P35*$V$14-$V$15))</f>
         <v>1.2245488615868059</v>
       </c>
       <c r="R35" s="16">
-        <f>M35*$Y$28/(N35*$Y$27)</f>
+        <f>M35*$U$15/(N35*$U$14)</f>
         <v>1.1026596825829091</v>
       </c>
       <c r="S35" s="16">
-        <f>-$Y$30/LN((R35-1)/(R35*$Z$27-$Z$28))</f>
+        <f>-$U$17/LN((R35-1)/(R35*$V$14-$V$15))</f>
         <v>1.2245488615868034</v>
       </c>
-      <c r="U35" s="3">
+      <c r="U35" s="16">
         <v>1.2245488615868163</v>
       </c>
       <c r="W35" s="3">
-        <f>M35-0.2</f>
+        <f t="shared" si="4"/>
         <v>0.8</v>
       </c>
       <c r="X35" s="3">
-        <f>Y28/Y27</f>
-        <v>4.9756642380027891</v>
+        <f t="shared" si="5"/>
+        <v>0.5</v>
       </c>
       <c r="Y35" s="3">
-        <f>X35/T2</f>
-        <v>1.0497181936714743</v>
+        <f t="shared" si="6"/>
+        <v>1.3778865608202484</v>
       </c>
     </row>
     <row r="36" spans="11:25">
@@ -7255,35 +7650,43 @@
         <v>45.998168498168496</v>
       </c>
       <c r="M36" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N36" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.5756733669401615</v>
       </c>
       <c r="P36" s="16">
-        <f>K36*$Y$28/(L36*$Y$27)</f>
+        <f>K36*$U$15/(L36*$U$14)</f>
         <v>1.3915320912717071</v>
       </c>
       <c r="Q36" s="16">
-        <f>-$Y$30/LN((P36-1)/(P36*$Z$27-$Z$28))</f>
+        <f>-$U$17/LN((P36-1)/(P36*$V$14-$V$15))</f>
         <v>4.5022730604685011</v>
       </c>
       <c r="R36" s="16">
-        <f>M36*$Y$28/(N36*$Y$27)</f>
+        <f>M36*$U$15/(N36*$U$14)</f>
         <v>1.3915320912717071</v>
       </c>
       <c r="S36" s="16">
-        <f>-$Y$30/LN((R36-1)/(R36*$Z$27-$Z$28))</f>
+        <f>-$U$17/LN((R36-1)/(R36*$V$14-$V$15))</f>
         <v>4.5022730604685011</v>
       </c>
-      <c r="U36" s="3">
+      <c r="U36" s="16">
         <v>4.5022730604685153</v>
       </c>
       <c r="W36" s="3">
-        <f>M36-0.2</f>
+        <f t="shared" si="4"/>
         <v>0.8</v>
+      </c>
+      <c r="X36" s="3">
+        <f t="shared" si="5"/>
+        <v>0.5</v>
+      </c>
+      <c r="Y36" s="3">
+        <f t="shared" si="6"/>
+        <v>4.6276981722017112</v>
       </c>
     </row>
     <row r="37" spans="11:25">
@@ -7297,6 +7700,7 @@
       <c r="Q37" s="16"/>
       <c r="R37" s="16"/>
       <c r="S37" s="16"/>
+      <c r="U37" s="16"/>
     </row>
     <row r="38" spans="11:25">
       <c r="K38" s="6">
@@ -7306,35 +7710,43 @@
         <v>43.316326530612244</v>
       </c>
       <c r="M38" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N38" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.2225965525269222</v>
       </c>
       <c r="P38" s="16">
-        <f>K38*$Y$28/(L38*$Y$27)</f>
+        <f>K38*$U$15/(L38*$U$14)</f>
         <v>1.1783423247066334</v>
       </c>
       <c r="Q38" s="16">
-        <f>-$Y$30/LN((P38-1)/(P38*$Z$27-$Z$28))</f>
+        <f>-$U$17/LN((P38-1)/(P38*$V$14-$V$15))</f>
         <v>2.0759804104281954</v>
       </c>
       <c r="R38" s="16">
-        <f>M38*$Y$28/(N38*$Y$27)</f>
+        <f>M38*$U$15/(N38*$U$14)</f>
         <v>1.1783423247066334</v>
       </c>
       <c r="S38" s="16">
-        <f>-$Y$30/LN((R38-1)/(R38*$Z$27-$Z$28))</f>
+        <f>-$U$17/LN((R38-1)/(R38*$V$14-$V$15))</f>
         <v>2.0759804104281954</v>
       </c>
-      <c r="U38" s="3">
+      <c r="U38" s="16">
         <v>2.0759804104282051</v>
       </c>
       <c r="W38" s="3">
-        <f>M38-0.2</f>
+        <f t="shared" ref="W38:X45" si="7">M38-0.2</f>
         <v>0.8</v>
+      </c>
+      <c r="X38" s="3">
+        <f t="shared" si="5"/>
+        <v>0.5</v>
+      </c>
+      <c r="Y38" s="3">
+        <f t="shared" si="6"/>
+        <v>2.2217351239820298</v>
       </c>
     </row>
     <row r="39" spans="11:25">
@@ -7345,35 +7757,43 @@
         <v>60.157142857142851</v>
       </c>
       <c r="M39" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N39" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.5787113870193199</v>
       </c>
       <c r="P39" s="16">
-        <f>K39*$Y$28/(L39*$Y$27)</f>
+        <f>K39*$U$15/(L39*$U$14)</f>
         <v>1.0866953204582479</v>
       </c>
       <c r="Q39" s="16">
-        <f>-$Y$30/LN((P39-1)/(P39*$Z$27-$Z$28))</f>
+        <f>-$U$17/LN((P39-1)/(P39*$V$14-$V$15))</f>
         <v>1.045487730213289</v>
       </c>
       <c r="R39" s="16">
-        <f>M39*$Y$28/(N39*$Y$27)</f>
+        <f>M39*$U$15/(N39*$U$14)</f>
         <v>1.0866953204582481</v>
       </c>
       <c r="S39" s="16">
-        <f>-$Y$30/LN((R39-1)/(R39*$Z$27-$Z$28))</f>
+        <f>-$U$17/LN((R39-1)/(R39*$V$14-$V$15))</f>
         <v>1.0454877302132917</v>
       </c>
-      <c r="U39" s="3">
+      <c r="U39" s="16">
         <v>1.0454877302133012</v>
       </c>
       <c r="W39" s="3">
-        <f>M39-0.2</f>
+        <f t="shared" si="7"/>
         <v>0.8</v>
+      </c>
+      <c r="X39" s="3">
+        <f t="shared" si="5"/>
+        <v>0.5</v>
+      </c>
+      <c r="Y39" s="3">
+        <f t="shared" si="6"/>
+        <v>1.200565308077219</v>
       </c>
     </row>
     <row r="40" spans="11:25">
@@ -7384,35 +7804,43 @@
         <v>55.175097276264601</v>
       </c>
       <c r="M40" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N40" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.4786745901367118</v>
       </c>
       <c r="P40" s="16">
-        <f>K40*$Y$28/(L40*$Y$27)</f>
+        <f>K40*$U$15/(L40*$U$14)</f>
         <v>1.1109680191904514</v>
       </c>
       <c r="Q40" s="16">
-        <f>-$Y$30/LN((P40-1)/(P40*$Z$27-$Z$28))</f>
+        <f>-$U$17/LN((P40-1)/(P40*$V$14-$V$15))</f>
         <v>1.3177997023817716</v>
       </c>
       <c r="R40" s="16">
-        <f>M40*$Y$28/(N40*$Y$27)</f>
+        <f>M40*$U$15/(N40*$U$14)</f>
         <v>1.1109680191904514</v>
       </c>
       <c r="S40" s="16">
-        <f>-$Y$30/LN((R40-1)/(R40*$Z$27-$Z$28))</f>
+        <f>-$U$17/LN((R40-1)/(R40*$V$14-$V$15))</f>
         <v>1.3177997023817716</v>
       </c>
-      <c r="U40" s="3">
+      <c r="U40" s="16">
         <v>1.3177997023817838</v>
       </c>
       <c r="W40" s="3">
-        <f>M40-0.2</f>
+        <f t="shared" si="7"/>
         <v>0.8</v>
+      </c>
+      <c r="X40" s="3">
+        <f t="shared" si="5"/>
+        <v>0.5</v>
+      </c>
+      <c r="Y40" s="3">
+        <f t="shared" si="6"/>
+        <v>1.4702631825429489</v>
       </c>
     </row>
     <row r="41" spans="11:25">
@@ -7423,35 +7851,43 @@
         <v>31.387478849407781</v>
       </c>
       <c r="M41" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N41" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.9322286820893075</v>
       </c>
       <c r="P41" s="16">
-        <f>K41*$Y$28/(L41*$Y$27)</f>
+        <f>K41*$U$15/(L41*$U$14)</f>
         <v>1.2653547492459349</v>
       </c>
       <c r="Q41" s="16">
-        <f>-$Y$30/LN((P41-1)/(P41*$Z$27-$Z$28))</f>
+        <f>-$U$17/LN((P41-1)/(P41*$V$14-$V$15))</f>
         <v>3.0610911009201853</v>
       </c>
       <c r="R41" s="16">
-        <f>M41*$Y$28/(N41*$Y$27)</f>
+        <f>M41*$U$15/(N41*$U$14)</f>
         <v>1.2653547492459349</v>
       </c>
       <c r="S41" s="16">
-        <f>-$Y$30/LN((R41-1)/(R41*$Z$27-$Z$28))</f>
+        <f>-$U$17/LN((R41-1)/(R41*$V$14-$V$15))</f>
         <v>3.0610911009201853</v>
       </c>
-      <c r="U41" s="3">
+      <c r="U41" s="16">
         <v>3.061091100920192</v>
       </c>
       <c r="W41" s="3">
-        <f>M41-0.2</f>
+        <f t="shared" si="7"/>
         <v>0.8</v>
+      </c>
+      <c r="X41" s="3">
+        <f t="shared" si="5"/>
+        <v>0.5</v>
+      </c>
+      <c r="Y41" s="3">
+        <f t="shared" si="6"/>
+        <v>3.198524609666793</v>
       </c>
     </row>
     <row r="42" spans="11:25">
@@ -7462,35 +7898,43 @@
         <v>32.173174872665534</v>
       </c>
       <c r="M42" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N42" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.7410668456587826</v>
       </c>
       <c r="P42" s="16">
-        <f>K42*$Y$28/(L42*$Y$27)</f>
+        <f>K42*$U$15/(L42*$U$14)</f>
         <v>1.3300121177403341</v>
       </c>
       <c r="Q42" s="16">
-        <f>-$Y$30/LN((P42-1)/(P42*$Z$27-$Z$28))</f>
+        <f>-$U$17/LN((P42-1)/(P42*$V$14-$V$15))</f>
         <v>3.7976968502088377</v>
       </c>
       <c r="R42" s="16">
-        <f>M42*$Y$28/(N42*$Y$27)</f>
+        <f>M42*$U$15/(N42*$U$14)</f>
         <v>1.3300121177403341</v>
       </c>
       <c r="S42" s="16">
-        <f>-$Y$30/LN((R42-1)/(R42*$Z$27-$Z$28))</f>
+        <f>-$U$17/LN((R42-1)/(R42*$V$14-$V$15))</f>
         <v>3.7976968502088377</v>
       </c>
-      <c r="U42" s="3">
+      <c r="U42" s="16">
         <v>3.7976968502088173</v>
       </c>
       <c r="W42" s="3">
-        <f>M42-0.2</f>
+        <f t="shared" si="7"/>
         <v>0.8</v>
+      </c>
+      <c r="X42" s="3">
+        <f t="shared" si="5"/>
+        <v>0.5</v>
+      </c>
+      <c r="Y42" s="3">
+        <f t="shared" si="6"/>
+        <v>3.9289860295100238</v>
       </c>
     </row>
     <row r="43" spans="11:25">
@@ -7501,35 +7945,43 @@
         <v>21.189115646258507</v>
       </c>
       <c r="M43" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N43" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.5155919631758685</v>
       </c>
       <c r="P43" s="16">
-        <f>K43*$Y$28/(L43*$Y$27)</f>
+        <f>K43*$U$15/(L43*$U$14)</f>
         <v>1.4153133498200228</v>
       </c>
       <c r="Q43" s="16">
-        <f>-$Y$30/LN((P43-1)/(P43*$Z$27-$Z$28))</f>
+        <f>-$U$17/LN((P43-1)/(P43*$V$14-$V$15))</f>
         <v>4.7756156281657471</v>
       </c>
       <c r="R43" s="16">
-        <f>M43*$Y$28/(N43*$Y$27)</f>
+        <f>M43*$U$15/(N43*$U$14)</f>
         <v>1.4153133498200228</v>
       </c>
       <c r="S43" s="16">
-        <f>-$Y$30/LN((R43-1)/(R43*$Z$27-$Z$28))</f>
+        <f>-$U$17/LN((R43-1)/(R43*$V$14-$V$15))</f>
         <v>4.7756156281657471</v>
       </c>
-      <c r="U43" s="3">
+      <c r="U43" s="16">
         <v>4.7756156281658271</v>
       </c>
       <c r="W43" s="3">
-        <f>M43-0.2</f>
+        <f t="shared" si="7"/>
         <v>0.8</v>
+      </c>
+      <c r="X43" s="3">
+        <f t="shared" si="5"/>
+        <v>0.5</v>
+      </c>
+      <c r="Y43" s="3">
+        <f t="shared" si="6"/>
+        <v>4.8987652257913643</v>
       </c>
     </row>
     <row r="44" spans="11:25">
@@ -7540,35 +7992,43 @@
         <v>51.16115702479339</v>
       </c>
       <c r="M44" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N44" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.1774399116059011</v>
       </c>
       <c r="P44" s="16">
-        <f>K44*$Y$28/(L44*$Y$27)</f>
+        <f>K44*$U$15/(L44*$U$14)</f>
         <v>1.5659349590935463</v>
       </c>
       <c r="Q44" s="16">
-        <f>-$Y$30/LN((P44-1)/(P44*$Z$27-$Z$28))</f>
+        <f>-$U$17/LN((P44-1)/(P44*$V$14-$V$15))</f>
         <v>6.519728458894841</v>
       </c>
       <c r="R44" s="16">
-        <f>M44*$Y$28/(N44*$Y$27)</f>
+        <f>M44*$U$15/(N44*$U$14)</f>
         <v>1.5659349590935465</v>
       </c>
       <c r="S44" s="16">
-        <f>-$Y$30/LN((R44-1)/(R44*$Z$27-$Z$28))</f>
+        <f>-$U$17/LN((R44-1)/(R44*$V$14-$V$15))</f>
         <v>6.519728458894841</v>
       </c>
-      <c r="U44" s="3">
+      <c r="U44" s="16">
         <v>6.5197284588949005</v>
       </c>
       <c r="W44" s="3">
-        <f>M44-0.2</f>
+        <f t="shared" si="7"/>
         <v>0.8</v>
+      </c>
+      <c r="X44" s="3">
+        <f t="shared" si="5"/>
+        <v>0.5</v>
+      </c>
+      <c r="Y44" s="3">
+        <f t="shared" si="6"/>
+        <v>6.6283127156830597</v>
       </c>
     </row>
     <row r="45" spans="11:25">
@@ -7579,35 +8039,43 @@
         <v>27.604724409448821</v>
       </c>
       <c r="M45" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N45" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.0956776505992174</v>
       </c>
       <c r="P45" s="16">
-        <f>K45*$Y$28/(L45*$Y$27)</f>
+        <f>K45*$U$15/(L45*$U$14)</f>
         <v>1.2148573844122781</v>
       </c>
       <c r="Q45" s="16">
-        <f>-$Y$30/LN((P45-1)/(P45*$Z$27-$Z$28))</f>
+        <f>-$U$17/LN((P45-1)/(P45*$V$14-$V$15))</f>
         <v>2.488538187070489</v>
       </c>
       <c r="R45" s="16">
-        <f>M45*$Y$28/(N45*$Y$27)</f>
+        <f>M45*$U$15/(N45*$U$14)</f>
         <v>1.2148573844122781</v>
       </c>
       <c r="S45" s="16">
-        <f>-$Y$30/LN((R45-1)/(R45*$Z$27-$Z$28))</f>
+        <f>-$U$17/LN((R45-1)/(R45*$V$14-$V$15))</f>
         <v>2.488538187070489</v>
       </c>
-      <c r="U45" s="3">
+      <c r="U45" s="16">
         <v>2.4885381870705521</v>
       </c>
       <c r="W45" s="3">
-        <f>M45-0.2</f>
+        <f t="shared" si="7"/>
         <v>0.8</v>
+      </c>
+      <c r="X45" s="3">
+        <f t="shared" si="5"/>
+        <v>0.5</v>
+      </c>
+      <c r="Y45" s="3">
+        <f t="shared" si="6"/>
+        <v>2.6307823880651098</v>
       </c>
     </row>
     <row r="46" spans="11:25">
@@ -7621,6 +8089,7 @@
       <c r="Q46" s="16"/>
       <c r="R46" s="16"/>
       <c r="S46" s="16"/>
+      <c r="U46" s="16"/>
     </row>
     <row r="47" spans="11:25">
       <c r="K47" s="6">
@@ -7630,35 +8099,43 @@
         <v>30.030456852791875</v>
       </c>
       <c r="M47" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="N47" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.7556266931751354</v>
       </c>
       <c r="P47" s="16">
-        <f>K47*$Y$28/(L47*$Y$27)</f>
+        <f>K47*$U$15/(L47*$U$14)</f>
         <v>1.3248559147384777</v>
       </c>
       <c r="Q47" s="16">
-        <f>-$Y$30/LN((P47-1)/(P47*$Z$27-$Z$28))</f>
+        <f>-$U$17/LN((P47-1)/(P47*$V$14-$V$15))</f>
         <v>3.7388090681306001</v>
       </c>
       <c r="R47" s="16">
-        <f>M47*$Y$28/(N47*$Y$27)</f>
+        <f>M47*$U$15/(N47*$U$14)</f>
         <v>1.324855914738478</v>
       </c>
       <c r="S47" s="16">
-        <f>-$Y$30/LN((R47-1)/(R47*$Z$27-$Z$28))</f>
+        <f>-$U$17/LN((R47-1)/(R47*$V$14-$V$15))</f>
         <v>3.7388090681306001</v>
       </c>
-      <c r="U47" s="3">
+      <c r="U47" s="16">
         <v>3.7388090681306001</v>
       </c>
       <c r="W47" s="3">
         <f>M47-0.2</f>
         <v>0.8</v>
+      </c>
+      <c r="X47" s="3">
+        <f t="shared" si="5"/>
+        <v>0.5</v>
+      </c>
+      <c r="Y47" s="3">
+        <f t="shared" si="6"/>
+        <v>3.8705886023000229</v>
       </c>
     </row>
     <row r="49" spans="13:19">
@@ -7717,7 +8194,7 @@
   <dimension ref="A1:AI26"/>
   <sheetViews>
     <sheetView topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AD23" sqref="AD23"/>
+      <selection activeCell="AD9" sqref="AD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10727,67 +11204,67 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E23">
-    <cfRule type="cellIs" dxfId="108" priority="20" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="106" priority="20" operator="greaterThan">
       <formula>$D2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C23">
-    <cfRule type="cellIs" dxfId="107" priority="19" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="105" priority="19" operator="greaterThan">
       <formula>$B2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G23">
-    <cfRule type="cellIs" dxfId="106" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="104" priority="14" operator="greaterThan">
       <formula>$F2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I23">
-    <cfRule type="cellIs" dxfId="105" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="103" priority="13" operator="greaterThan">
       <formula>$H2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K23">
-    <cfRule type="cellIs" dxfId="104" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="102" priority="12" operator="greaterThan">
       <formula>$J2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M23 Z2:AA23">
-    <cfRule type="cellIs" dxfId="103" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="101" priority="11" operator="greaterThan">
       <formula>$L2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC2:AI23">
-    <cfRule type="cellIs" dxfId="102" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="100" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O23">
-    <cfRule type="cellIs" dxfId="101" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="99" priority="7" operator="greaterThan">
       <formula>$N2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q23">
-    <cfRule type="cellIs" dxfId="100" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="98" priority="6" operator="greaterThan">
       <formula>$P2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S23">
-    <cfRule type="cellIs" dxfId="99" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="97" priority="4" operator="greaterThan">
       <formula>$R2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2:U23">
-    <cfRule type="cellIs" dxfId="98" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="96" priority="3" operator="greaterThan">
       <formula>$T2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W2:W23">
-    <cfRule type="cellIs" dxfId="97" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="95" priority="2" operator="greaterThan">
       <formula>$V2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y2:Y23">
-    <cfRule type="cellIs" dxfId="96" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="94" priority="1" operator="greaterThan">
       <formula>$X2</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>